<commit_message>
Dettagliata gestione errore per i casi segnalati
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#MEDINFORMATICAXX/Medinformatica/MediStudio/24.2.28.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111#MEDINFORMATICAXX/Medinformatica/MediStudio/24.2.28.0/report-checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE\it-fse-accreditamento\GATEWAY\S1#111#MEDINFORMATICAXX\Medinformatica\MediStudio\24.2.28.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\__DEV__\FSE\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902A2E42-8D0F-4DAA-BE6A-DA1A4681FB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="2"/>
+    <workbookView xWindow="2970" yWindow="450" windowWidth="27060" windowHeight="15150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -27,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="903">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4805,9 +4806,6 @@
     <t>Errore di comunicazione (timeout)</t>
   </si>
   <si>
-    <t>L'utente è invitato a riprovare la validazione in un secondo momento e a contattare l'assistenza qualora l'errore persista.</t>
-  </si>
-  <si>
     <t>Di fatto non potrà mai succedere di non valorizzare nel JWT il campo "purpose_of_use"</t>
   </si>
   <si>
@@ -4815,12 +4813,18 @@
   </si>
   <si>
     <t>L'errore appare all'utente in fase di invio del referto in modo che possa correggerne la causa e ritentare un nuovo invio dopo la correzione.</t>
+  </si>
+  <si>
+    <t>L'utente è invitato, tramite MsgBox, a riprovare la validazione in un secondo momento e a contattare l'assistenza qualora l'errore persista. Medinformatica, consultando i log, potrà intervenire.</t>
+  </si>
+  <si>
+    <t>L'utente riceve questo MsgBox "Impossibile comunicare con il Gateway FSE. Riprovare in secondo momento, e contattare l'assistenza qualora l'errore persista."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -5156,9 +5160,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+  <cellXfs count="65">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5265,9 +5269,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -5288,9 +5289,27 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -5308,24 +5327,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5382,12 +5383,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -5410,18 +5411,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" name="ESITO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ESITO"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="B1:B3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B1:B3">
   <tableColumns count="1">
-    <tableColumn id="1" name="APPLICABILITA'"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="APPLICABILITA'"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5627,7 +5628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5706,7 +5707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5820,15 +5821,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="M22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5845,12 +5846,12 @@
     <col min="10" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="48.28515625" customWidth="1"/>
     <col min="12" max="13" width="36.42578125" customWidth="1"/>
-    <col min="14" max="14" width="36.42578125" style="62" customWidth="1"/>
+    <col min="14" max="14" width="36.42578125" style="49" customWidth="1"/>
     <col min="15" max="15" width="36.42578125" customWidth="1"/>
-    <col min="16" max="16" width="43.140625" style="62" customWidth="1"/>
+    <col min="16" max="16" width="73" style="49" customWidth="1"/>
     <col min="17" max="17" width="33.140625" customWidth="1"/>
     <col min="18" max="18" width="36.42578125" customWidth="1"/>
-    <col min="19" max="19" width="31.85546875" style="62" customWidth="1"/>
+    <col min="19" max="19" width="31.85546875" style="49" customWidth="1"/>
     <col min="20" max="20" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5864,23 +5865,23 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="60"/>
+      <c r="N1" s="47"/>
       <c r="O1" s="15"/>
-      <c r="P1" s="60"/>
+      <c r="P1" s="47"/>
       <c r="Q1" s="15"/>
       <c r="R1" s="16"/>
-      <c r="S1" s="63"/>
+      <c r="S1" s="50"/>
       <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="51"/>
+      <c r="D2" s="56"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -5889,23 +5890,23 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="60"/>
+      <c r="N2" s="47"/>
       <c r="O2" s="15"/>
-      <c r="P2" s="60"/>
+      <c r="P2" s="47"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="16"/>
-      <c r="S2" s="63"/>
+      <c r="S2" s="50"/>
       <c r="T2" s="17"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="59"/>
+      <c r="C3" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="56"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -5914,21 +5915,21 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
-      <c r="N3" s="60"/>
+      <c r="N3" s="47"/>
       <c r="O3" s="15"/>
-      <c r="P3" s="60"/>
+      <c r="P3" s="47"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="16"/>
-      <c r="S3" s="63"/>
+      <c r="S3" s="50"/>
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="59" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="51"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="6"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -5938,21 +5939,21 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
-      <c r="N4" s="60"/>
+      <c r="N4" s="47"/>
       <c r="O4" s="15"/>
-      <c r="P4" s="60"/>
+      <c r="P4" s="47"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="16"/>
-      <c r="S4" s="63"/>
+      <c r="S4" s="50"/>
       <c r="T4" s="17"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="57"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="59" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="56"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -5961,17 +5962,17 @@
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
-      <c r="N5" s="60"/>
+      <c r="N5" s="47"/>
       <c r="O5" s="15"/>
-      <c r="P5" s="60"/>
+      <c r="P5" s="47"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="16"/>
-      <c r="S5" s="63"/>
+      <c r="S5" s="50"/>
       <c r="T5" s="17"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="18"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -5981,12 +5982,12 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
-      <c r="N6" s="60"/>
+      <c r="N6" s="47"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="60"/>
+      <c r="P6" s="47"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="63"/>
+      <c r="S6" s="50"/>
       <c r="T6" s="17"/>
     </row>
     <row r="7" spans="1:20" ht="14.25" customHeight="1">
@@ -6001,12 +6002,12 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
-      <c r="N7" s="60"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="15"/>
-      <c r="P7" s="60"/>
+      <c r="P7" s="47"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="16"/>
-      <c r="S7" s="63"/>
+      <c r="S7" s="50"/>
       <c r="T7" s="17"/>
     </row>
     <row r="8" spans="1:20" ht="14.25" customHeight="1">
@@ -6018,12 +6019,12 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="60"/>
+      <c r="N8" s="47"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="60"/>
+      <c r="P8" s="47"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="16"/>
-      <c r="S8" s="63"/>
+      <c r="S8" s="50"/>
       <c r="T8" s="17"/>
     </row>
     <row r="9" spans="1:20" ht="14.25" customHeight="1">
@@ -6066,13 +6067,13 @@
       <c r="M9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="65" t="s">
+      <c r="N9" s="52" t="s">
         <v>41</v>
       </c>
       <c r="O9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="65" t="s">
+      <c r="P9" s="52" t="s">
         <v>43</v>
       </c>
       <c r="Q9" s="20" t="s">
@@ -6081,7 +6082,7 @@
       <c r="R9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="S9" s="65" t="s">
+      <c r="S9" s="52" t="s">
         <v>46</v>
       </c>
       <c r="T9" s="20" t="s">
@@ -7148,19 +7149,19 @@
       <c r="M38" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N38" s="61" t="s">
+      <c r="N38" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O38" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P38" s="61" t="s">
-        <v>898</v>
+      <c r="P38" s="48" t="s">
+        <v>901</v>
       </c>
       <c r="Q38" s="27"/>
       <c r="R38" s="28"/>
-      <c r="S38" s="64" t="s">
-        <v>899</v>
+      <c r="S38" s="51" t="s">
+        <v>898</v>
       </c>
       <c r="T38" s="30" t="s">
         <v>115</v>
@@ -7176,7 +7177,7 @@
       <c r="C39" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="23" t="s">
         <v>126</v>
       </c>
       <c r="E39" s="24" t="s">
@@ -7204,19 +7205,19 @@
       <c r="M39" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N39" s="61" t="s">
+      <c r="N39" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O39" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P39" s="61" t="s">
-        <v>898</v>
+      <c r="P39" s="48" t="s">
+        <v>901</v>
       </c>
       <c r="Q39" s="27"/>
       <c r="R39" s="28"/>
-      <c r="S39" s="64" t="s">
-        <v>899</v>
+      <c r="S39" s="51" t="s">
+        <v>898</v>
       </c>
       <c r="T39" s="30" t="s">
         <v>115</v>
@@ -7476,19 +7477,19 @@
       <c r="M46" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N46" s="61" t="s">
+      <c r="N46" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P46" s="61" t="s">
-        <v>898</v>
+      <c r="P46" s="48" t="s">
+        <v>901</v>
       </c>
       <c r="Q46" s="27"/>
       <c r="R46" s="28"/>
-      <c r="S46" s="64" t="s">
-        <v>900</v>
+      <c r="S46" s="51" t="s">
+        <v>899</v>
       </c>
       <c r="T46" s="30" t="s">
         <v>115</v>
@@ -7504,7 +7505,7 @@
       <c r="C47" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D47" s="40" t="s">
+      <c r="D47" s="23" t="s">
         <v>144</v>
       </c>
       <c r="E47" s="24" t="s">
@@ -7532,19 +7533,19 @@
       <c r="M47" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N47" s="61" t="s">
+      <c r="N47" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O47" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P47" s="61" t="s">
-        <v>898</v>
+      <c r="P47" s="48" t="s">
+        <v>901</v>
       </c>
       <c r="Q47" s="27"/>
       <c r="R47" s="28"/>
-      <c r="S47" s="64" t="s">
-        <v>900</v>
+      <c r="S47" s="51" t="s">
+        <v>899</v>
       </c>
       <c r="T47" s="30" t="s">
         <v>115</v>
@@ -7802,18 +7803,18 @@
       <c r="M54" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N54" s="61" t="s">
+      <c r="N54" s="48" t="s">
         <v>897</v>
       </c>
       <c r="O54" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P54" s="61" t="s">
-        <v>898</v>
+      <c r="P54" s="48" t="s">
+        <v>902</v>
       </c>
       <c r="Q54" s="27"/>
       <c r="R54" s="28"/>
-      <c r="S54" s="64"/>
+      <c r="S54" s="51"/>
       <c r="T54" s="30" t="s">
         <v>115</v>
       </c>
@@ -7848,18 +7849,18 @@
       <c r="M55" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N55" s="61" t="s">
+      <c r="N55" s="48" t="s">
         <v>897</v>
       </c>
       <c r="O55" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P55" s="61" t="s">
-        <v>898</v>
+      <c r="P55" s="48" t="s">
+        <v>902</v>
       </c>
       <c r="Q55" s="27"/>
       <c r="R55" s="28"/>
-      <c r="S55" s="64"/>
+      <c r="S55" s="51"/>
       <c r="T55" s="30" t="s">
         <v>115</v>
       </c>
@@ -8882,18 +8883,18 @@
       <c r="M83" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N83" s="61" t="s">
+      <c r="N83" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O83" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P83" s="61" t="s">
-        <v>901</v>
+      <c r="P83" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q83" s="27"/>
       <c r="R83" s="28"/>
-      <c r="S83" s="64"/>
+      <c r="S83" s="51"/>
       <c r="T83" s="30" t="s">
         <v>115</v>
       </c>
@@ -8974,18 +8975,18 @@
       <c r="M85" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N85" s="61" t="s">
+      <c r="N85" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O85" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P85" s="61" t="s">
-        <v>901</v>
+      <c r="P85" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q85" s="27"/>
       <c r="R85" s="28"/>
-      <c r="S85" s="64"/>
+      <c r="S85" s="51"/>
       <c r="T85" s="30" t="s">
         <v>115</v>
       </c>
@@ -9028,18 +9029,18 @@
       <c r="M86" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N86" s="61" t="s">
+      <c r="N86" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O86" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P86" s="61" t="s">
-        <v>901</v>
+      <c r="P86" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q86" s="27"/>
       <c r="R86" s="28"/>
-      <c r="S86" s="64"/>
+      <c r="S86" s="51"/>
       <c r="T86" s="30" t="s">
         <v>115</v>
       </c>
@@ -11494,7 +11495,7 @@
       <c r="C154" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D154" s="40" t="s">
+      <c r="D154" s="23" t="s">
         <v>371</v>
       </c>
       <c r="E154" s="24" t="s">
@@ -11690,7 +11691,7 @@
       <c r="C159" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D159" s="40" t="s">
+      <c r="D159" s="23" t="s">
         <v>383</v>
       </c>
       <c r="E159" s="24" t="s">
@@ -11718,18 +11719,18 @@
       <c r="M159" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N159" s="61" t="s">
+      <c r="N159" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O159" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P159" s="61" t="s">
-        <v>901</v>
+      <c r="P159" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q159" s="27"/>
       <c r="R159" s="28"/>
-      <c r="S159" s="64"/>
+      <c r="S159" s="51"/>
       <c r="T159" s="30" t="s">
         <v>115</v>
       </c>
@@ -11782,7 +11783,7 @@
       <c r="C161" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D161" s="40" t="s">
+      <c r="D161" s="23" t="s">
         <v>389</v>
       </c>
       <c r="E161" s="24" t="s">
@@ -11810,18 +11811,18 @@
       <c r="M161" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N161" s="61" t="s">
+      <c r="N161" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O161" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P161" s="61" t="s">
-        <v>901</v>
+      <c r="P161" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q161" s="27"/>
       <c r="R161" s="28"/>
-      <c r="S161" s="64"/>
+      <c r="S161" s="51"/>
       <c r="T161" s="30" t="s">
         <v>115</v>
       </c>
@@ -11836,7 +11837,7 @@
       <c r="C162" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D162" s="40" t="s">
+      <c r="D162" s="23" t="s">
         <v>393</v>
       </c>
       <c r="E162" s="24" t="s">
@@ -11864,18 +11865,18 @@
       <c r="M162" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="N162" s="61" t="s">
+      <c r="N162" s="48" t="s">
         <v>124</v>
       </c>
       <c r="O162" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="P162" s="61" t="s">
-        <v>901</v>
+      <c r="P162" s="48" t="s">
+        <v>900</v>
       </c>
       <c r="Q162" s="27"/>
       <c r="R162" s="28"/>
-      <c r="S162" s="64"/>
+      <c r="S162" s="51"/>
       <c r="T162" s="30" t="s">
         <v>115</v>
       </c>
@@ -19774,7 +19775,7 @@
       <c r="C381" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D381" s="40" t="s">
+      <c r="D381" s="23" t="s">
         <v>836</v>
       </c>
       <c r="E381" s="24" t="s">
@@ -19889,12 +19890,12 @@
       <c r="K384" s="15"/>
       <c r="L384" s="15"/>
       <c r="M384" s="15"/>
-      <c r="N384" s="60"/>
+      <c r="N384" s="47"/>
       <c r="O384" s="15"/>
-      <c r="P384" s="60"/>
+      <c r="P384" s="47"/>
       <c r="Q384" s="15"/>
       <c r="R384" s="16"/>
-      <c r="S384" s="63"/>
+      <c r="S384" s="50"/>
       <c r="T384" s="17"/>
     </row>
     <row r="385" spans="6:20" ht="14.25" customHeight="1">
@@ -19906,12 +19907,12 @@
       <c r="K385" s="15"/>
       <c r="L385" s="15"/>
       <c r="M385" s="15"/>
-      <c r="N385" s="60"/>
+      <c r="N385" s="47"/>
       <c r="O385" s="15"/>
-      <c r="P385" s="60"/>
+      <c r="P385" s="47"/>
       <c r="Q385" s="15"/>
       <c r="R385" s="16"/>
-      <c r="S385" s="63"/>
+      <c r="S385" s="50"/>
       <c r="T385" s="17"/>
     </row>
     <row r="386" spans="6:20" ht="14.25" customHeight="1">
@@ -19923,12 +19924,12 @@
       <c r="K386" s="15"/>
       <c r="L386" s="15"/>
       <c r="M386" s="15"/>
-      <c r="N386" s="60"/>
+      <c r="N386" s="47"/>
       <c r="O386" s="15"/>
-      <c r="P386" s="60"/>
+      <c r="P386" s="47"/>
       <c r="Q386" s="15"/>
       <c r="R386" s="16"/>
-      <c r="S386" s="63"/>
+      <c r="S386" s="50"/>
       <c r="T386" s="17"/>
     </row>
     <row r="387" spans="6:20" ht="14.25" customHeight="1">
@@ -19940,12 +19941,12 @@
       <c r="K387" s="15"/>
       <c r="L387" s="15"/>
       <c r="M387" s="15"/>
-      <c r="N387" s="60"/>
+      <c r="N387" s="47"/>
       <c r="O387" s="15"/>
-      <c r="P387" s="60"/>
+      <c r="P387" s="47"/>
       <c r="Q387" s="15"/>
       <c r="R387" s="16"/>
-      <c r="S387" s="63"/>
+      <c r="S387" s="50"/>
       <c r="T387" s="17"/>
     </row>
     <row r="388" spans="6:20" ht="14.25" customHeight="1">
@@ -19957,12 +19958,12 @@
       <c r="K388" s="15"/>
       <c r="L388" s="15"/>
       <c r="M388" s="15"/>
-      <c r="N388" s="60"/>
+      <c r="N388" s="47"/>
       <c r="O388" s="15"/>
-      <c r="P388" s="60"/>
+      <c r="P388" s="47"/>
       <c r="Q388" s="15"/>
       <c r="R388" s="16"/>
-      <c r="S388" s="63"/>
+      <c r="S388" s="50"/>
       <c r="T388" s="17"/>
     </row>
     <row r="389" spans="6:20" ht="14.25" customHeight="1">
@@ -19974,12 +19975,12 @@
       <c r="K389" s="15"/>
       <c r="L389" s="15"/>
       <c r="M389" s="15"/>
-      <c r="N389" s="60"/>
+      <c r="N389" s="47"/>
       <c r="O389" s="15"/>
-      <c r="P389" s="60"/>
+      <c r="P389" s="47"/>
       <c r="Q389" s="15"/>
       <c r="R389" s="16"/>
-      <c r="S389" s="63"/>
+      <c r="S389" s="50"/>
       <c r="T389" s="17"/>
     </row>
     <row r="390" spans="6:20" ht="14.25" customHeight="1">
@@ -19991,12 +19992,12 @@
       <c r="K390" s="15"/>
       <c r="L390" s="15"/>
       <c r="M390" s="15"/>
-      <c r="N390" s="60"/>
+      <c r="N390" s="47"/>
       <c r="O390" s="15"/>
-      <c r="P390" s="60"/>
+      <c r="P390" s="47"/>
       <c r="Q390" s="15"/>
       <c r="R390" s="16"/>
-      <c r="S390" s="63"/>
+      <c r="S390" s="50"/>
       <c r="T390" s="17"/>
     </row>
     <row r="391" spans="6:20" ht="14.25" customHeight="1">
@@ -20008,12 +20009,12 @@
       <c r="K391" s="15"/>
       <c r="L391" s="15"/>
       <c r="M391" s="15"/>
-      <c r="N391" s="60"/>
+      <c r="N391" s="47"/>
       <c r="O391" s="15"/>
-      <c r="P391" s="60"/>
+      <c r="P391" s="47"/>
       <c r="Q391" s="15"/>
       <c r="R391" s="16"/>
-      <c r="S391" s="63"/>
+      <c r="S391" s="50"/>
       <c r="T391" s="17"/>
     </row>
     <row r="392" spans="6:20" ht="14.25" customHeight="1">
@@ -20025,12 +20026,12 @@
       <c r="K392" s="15"/>
       <c r="L392" s="15"/>
       <c r="M392" s="15"/>
-      <c r="N392" s="60"/>
+      <c r="N392" s="47"/>
       <c r="O392" s="15"/>
-      <c r="P392" s="60"/>
+      <c r="P392" s="47"/>
       <c r="Q392" s="15"/>
       <c r="R392" s="16"/>
-      <c r="S392" s="63"/>
+      <c r="S392" s="50"/>
       <c r="T392" s="17"/>
     </row>
     <row r="393" spans="6:20" ht="14.25" customHeight="1">
@@ -20042,12 +20043,12 @@
       <c r="K393" s="15"/>
       <c r="L393" s="15"/>
       <c r="M393" s="15"/>
-      <c r="N393" s="60"/>
+      <c r="N393" s="47"/>
       <c r="O393" s="15"/>
-      <c r="P393" s="60"/>
+      <c r="P393" s="47"/>
       <c r="Q393" s="15"/>
       <c r="R393" s="16"/>
-      <c r="S393" s="63"/>
+      <c r="S393" s="50"/>
       <c r="T393" s="17"/>
     </row>
     <row r="394" spans="6:20" ht="14.25" customHeight="1">
@@ -20059,12 +20060,12 @@
       <c r="K394" s="15"/>
       <c r="L394" s="15"/>
       <c r="M394" s="15"/>
-      <c r="N394" s="60"/>
+      <c r="N394" s="47"/>
       <c r="O394" s="15"/>
-      <c r="P394" s="60"/>
+      <c r="P394" s="47"/>
       <c r="Q394" s="15"/>
       <c r="R394" s="16"/>
-      <c r="S394" s="63"/>
+      <c r="S394" s="50"/>
       <c r="T394" s="17"/>
     </row>
     <row r="395" spans="6:20" ht="14.25" customHeight="1">
@@ -20076,12 +20077,12 @@
       <c r="K395" s="15"/>
       <c r="L395" s="15"/>
       <c r="M395" s="15"/>
-      <c r="N395" s="60"/>
+      <c r="N395" s="47"/>
       <c r="O395" s="15"/>
-      <c r="P395" s="60"/>
+      <c r="P395" s="47"/>
       <c r="Q395" s="15"/>
       <c r="R395" s="16"/>
-      <c r="S395" s="63"/>
+      <c r="S395" s="50"/>
       <c r="T395" s="17"/>
     </row>
     <row r="396" spans="6:20" ht="14.25" customHeight="1">
@@ -20093,12 +20094,12 @@
       <c r="K396" s="15"/>
       <c r="L396" s="15"/>
       <c r="M396" s="15"/>
-      <c r="N396" s="60"/>
+      <c r="N396" s="47"/>
       <c r="O396" s="15"/>
-      <c r="P396" s="60"/>
+      <c r="P396" s="47"/>
       <c r="Q396" s="15"/>
       <c r="R396" s="16"/>
-      <c r="S396" s="63"/>
+      <c r="S396" s="50"/>
       <c r="T396" s="17"/>
     </row>
     <row r="397" spans="6:20" ht="14.25" customHeight="1">
@@ -20110,12 +20111,12 @@
       <c r="K397" s="15"/>
       <c r="L397" s="15"/>
       <c r="M397" s="15"/>
-      <c r="N397" s="60"/>
+      <c r="N397" s="47"/>
       <c r="O397" s="15"/>
-      <c r="P397" s="60"/>
+      <c r="P397" s="47"/>
       <c r="Q397" s="15"/>
       <c r="R397" s="16"/>
-      <c r="S397" s="63"/>
+      <c r="S397" s="50"/>
       <c r="T397" s="17"/>
     </row>
     <row r="398" spans="6:20" ht="14.25" customHeight="1">
@@ -20127,12 +20128,12 @@
       <c r="K398" s="15"/>
       <c r="L398" s="15"/>
       <c r="M398" s="15"/>
-      <c r="N398" s="60"/>
+      <c r="N398" s="47"/>
       <c r="O398" s="15"/>
-      <c r="P398" s="60"/>
+      <c r="P398" s="47"/>
       <c r="Q398" s="15"/>
       <c r="R398" s="16"/>
-      <c r="S398" s="63"/>
+      <c r="S398" s="50"/>
       <c r="T398" s="17"/>
     </row>
     <row r="399" spans="6:20" ht="14.25" customHeight="1">
@@ -20144,12 +20145,12 @@
       <c r="K399" s="15"/>
       <c r="L399" s="15"/>
       <c r="M399" s="15"/>
-      <c r="N399" s="60"/>
+      <c r="N399" s="47"/>
       <c r="O399" s="15"/>
-      <c r="P399" s="60"/>
+      <c r="P399" s="47"/>
       <c r="Q399" s="15"/>
       <c r="R399" s="16"/>
-      <c r="S399" s="63"/>
+      <c r="S399" s="50"/>
       <c r="T399" s="17"/>
     </row>
     <row r="400" spans="6:20" ht="14.25" customHeight="1">
@@ -20161,12 +20162,12 @@
       <c r="K400" s="15"/>
       <c r="L400" s="15"/>
       <c r="M400" s="15"/>
-      <c r="N400" s="60"/>
+      <c r="N400" s="47"/>
       <c r="O400" s="15"/>
-      <c r="P400" s="60"/>
+      <c r="P400" s="47"/>
       <c r="Q400" s="15"/>
       <c r="R400" s="16"/>
-      <c r="S400" s="63"/>
+      <c r="S400" s="50"/>
       <c r="T400" s="17"/>
     </row>
     <row r="401" spans="6:20" ht="14.25" customHeight="1">
@@ -20178,12 +20179,12 @@
       <c r="K401" s="15"/>
       <c r="L401" s="15"/>
       <c r="M401" s="15"/>
-      <c r="N401" s="60"/>
+      <c r="N401" s="47"/>
       <c r="O401" s="15"/>
-      <c r="P401" s="60"/>
+      <c r="P401" s="47"/>
       <c r="Q401" s="15"/>
       <c r="R401" s="16"/>
-      <c r="S401" s="63"/>
+      <c r="S401" s="50"/>
       <c r="T401" s="17"/>
     </row>
     <row r="402" spans="6:20" ht="14.25" customHeight="1">
@@ -20195,12 +20196,12 @@
       <c r="K402" s="15"/>
       <c r="L402" s="15"/>
       <c r="M402" s="15"/>
-      <c r="N402" s="60"/>
+      <c r="N402" s="47"/>
       <c r="O402" s="15"/>
-      <c r="P402" s="60"/>
+      <c r="P402" s="47"/>
       <c r="Q402" s="15"/>
       <c r="R402" s="16"/>
-      <c r="S402" s="63"/>
+      <c r="S402" s="50"/>
       <c r="T402" s="17"/>
     </row>
     <row r="403" spans="6:20" ht="14.25" customHeight="1">
@@ -20212,12 +20213,12 @@
       <c r="K403" s="15"/>
       <c r="L403" s="15"/>
       <c r="M403" s="15"/>
-      <c r="N403" s="60"/>
+      <c r="N403" s="47"/>
       <c r="O403" s="15"/>
-      <c r="P403" s="60"/>
+      <c r="P403" s="47"/>
       <c r="Q403" s="15"/>
       <c r="R403" s="16"/>
-      <c r="S403" s="63"/>
+      <c r="S403" s="50"/>
       <c r="T403" s="17"/>
     </row>
     <row r="404" spans="6:20" ht="14.25" customHeight="1">
@@ -20229,12 +20230,12 @@
       <c r="K404" s="15"/>
       <c r="L404" s="15"/>
       <c r="M404" s="15"/>
-      <c r="N404" s="60"/>
+      <c r="N404" s="47"/>
       <c r="O404" s="15"/>
-      <c r="P404" s="60"/>
+      <c r="P404" s="47"/>
       <c r="Q404" s="15"/>
       <c r="R404" s="16"/>
-      <c r="S404" s="63"/>
+      <c r="S404" s="50"/>
       <c r="T404" s="17"/>
     </row>
     <row r="405" spans="6:20" ht="14.25" customHeight="1">
@@ -20246,12 +20247,12 @@
       <c r="K405" s="15"/>
       <c r="L405" s="15"/>
       <c r="M405" s="15"/>
-      <c r="N405" s="60"/>
+      <c r="N405" s="47"/>
       <c r="O405" s="15"/>
-      <c r="P405" s="60"/>
+      <c r="P405" s="47"/>
       <c r="Q405" s="15"/>
       <c r="R405" s="16"/>
-      <c r="S405" s="63"/>
+      <c r="S405" s="50"/>
       <c r="T405" s="17"/>
     </row>
     <row r="406" spans="6:20" ht="14.25" customHeight="1">
@@ -20263,12 +20264,12 @@
       <c r="K406" s="15"/>
       <c r="L406" s="15"/>
       <c r="M406" s="15"/>
-      <c r="N406" s="60"/>
+      <c r="N406" s="47"/>
       <c r="O406" s="15"/>
-      <c r="P406" s="60"/>
+      <c r="P406" s="47"/>
       <c r="Q406" s="15"/>
       <c r="R406" s="16"/>
-      <c r="S406" s="63"/>
+      <c r="S406" s="50"/>
       <c r="T406" s="17"/>
     </row>
     <row r="407" spans="6:20" ht="14.25" customHeight="1">
@@ -20280,12 +20281,12 @@
       <c r="K407" s="15"/>
       <c r="L407" s="15"/>
       <c r="M407" s="15"/>
-      <c r="N407" s="60"/>
+      <c r="N407" s="47"/>
       <c r="O407" s="15"/>
-      <c r="P407" s="60"/>
+      <c r="P407" s="47"/>
       <c r="Q407" s="15"/>
       <c r="R407" s="16"/>
-      <c r="S407" s="63"/>
+      <c r="S407" s="50"/>
       <c r="T407" s="17"/>
     </row>
     <row r="408" spans="6:20" ht="14.25" customHeight="1">
@@ -20297,12 +20298,12 @@
       <c r="K408" s="15"/>
       <c r="L408" s="15"/>
       <c r="M408" s="15"/>
-      <c r="N408" s="60"/>
+      <c r="N408" s="47"/>
       <c r="O408" s="15"/>
-      <c r="P408" s="60"/>
+      <c r="P408" s="47"/>
       <c r="Q408" s="15"/>
       <c r="R408" s="16"/>
-      <c r="S408" s="63"/>
+      <c r="S408" s="50"/>
       <c r="T408" s="17"/>
     </row>
     <row r="409" spans="6:20" ht="14.25" customHeight="1">
@@ -20314,12 +20315,12 @@
       <c r="K409" s="15"/>
       <c r="L409" s="15"/>
       <c r="M409" s="15"/>
-      <c r="N409" s="60"/>
+      <c r="N409" s="47"/>
       <c r="O409" s="15"/>
-      <c r="P409" s="60"/>
+      <c r="P409" s="47"/>
       <c r="Q409" s="15"/>
       <c r="R409" s="16"/>
-      <c r="S409" s="63"/>
+      <c r="S409" s="50"/>
       <c r="T409" s="17"/>
     </row>
     <row r="410" spans="6:20" ht="14.25" customHeight="1">
@@ -20331,12 +20332,12 @@
       <c r="K410" s="15"/>
       <c r="L410" s="15"/>
       <c r="M410" s="15"/>
-      <c r="N410" s="60"/>
+      <c r="N410" s="47"/>
       <c r="O410" s="15"/>
-      <c r="P410" s="60"/>
+      <c r="P410" s="47"/>
       <c r="Q410" s="15"/>
       <c r="R410" s="16"/>
-      <c r="S410" s="63"/>
+      <c r="S410" s="50"/>
       <c r="T410" s="17"/>
     </row>
     <row r="411" spans="6:20" ht="14.25" customHeight="1">
@@ -20348,12 +20349,12 @@
       <c r="K411" s="15"/>
       <c r="L411" s="15"/>
       <c r="M411" s="15"/>
-      <c r="N411" s="60"/>
+      <c r="N411" s="47"/>
       <c r="O411" s="15"/>
-      <c r="P411" s="60"/>
+      <c r="P411" s="47"/>
       <c r="Q411" s="15"/>
       <c r="R411" s="16"/>
-      <c r="S411" s="63"/>
+      <c r="S411" s="50"/>
       <c r="T411" s="17"/>
     </row>
     <row r="412" spans="6:20" ht="14.25" customHeight="1">
@@ -20365,12 +20366,12 @@
       <c r="K412" s="15"/>
       <c r="L412" s="15"/>
       <c r="M412" s="15"/>
-      <c r="N412" s="60"/>
+      <c r="N412" s="47"/>
       <c r="O412" s="15"/>
-      <c r="P412" s="60"/>
+      <c r="P412" s="47"/>
       <c r="Q412" s="15"/>
       <c r="R412" s="16"/>
-      <c r="S412" s="63"/>
+      <c r="S412" s="50"/>
       <c r="T412" s="17"/>
     </row>
     <row r="413" spans="6:20" ht="14.25" customHeight="1">
@@ -20382,12 +20383,12 @@
       <c r="K413" s="15"/>
       <c r="L413" s="15"/>
       <c r="M413" s="15"/>
-      <c r="N413" s="60"/>
+      <c r="N413" s="47"/>
       <c r="O413" s="15"/>
-      <c r="P413" s="60"/>
+      <c r="P413" s="47"/>
       <c r="Q413" s="15"/>
       <c r="R413" s="16"/>
-      <c r="S413" s="63"/>
+      <c r="S413" s="50"/>
       <c r="T413" s="17"/>
     </row>
     <row r="414" spans="6:20" ht="14.25" customHeight="1">
@@ -20399,12 +20400,12 @@
       <c r="K414" s="15"/>
       <c r="L414" s="15"/>
       <c r="M414" s="15"/>
-      <c r="N414" s="60"/>
+      <c r="N414" s="47"/>
       <c r="O414" s="15"/>
-      <c r="P414" s="60"/>
+      <c r="P414" s="47"/>
       <c r="Q414" s="15"/>
       <c r="R414" s="16"/>
-      <c r="S414" s="63"/>
+      <c r="S414" s="50"/>
       <c r="T414" s="17"/>
     </row>
     <row r="415" spans="6:20" ht="14.25" customHeight="1">
@@ -20416,12 +20417,12 @@
       <c r="K415" s="15"/>
       <c r="L415" s="15"/>
       <c r="M415" s="15"/>
-      <c r="N415" s="60"/>
+      <c r="N415" s="47"/>
       <c r="O415" s="15"/>
-      <c r="P415" s="60"/>
+      <c r="P415" s="47"/>
       <c r="Q415" s="15"/>
       <c r="R415" s="16"/>
-      <c r="S415" s="63"/>
+      <c r="S415" s="50"/>
       <c r="T415" s="17"/>
     </row>
     <row r="416" spans="6:20" ht="14.25" customHeight="1">
@@ -20433,12 +20434,12 @@
       <c r="K416" s="15"/>
       <c r="L416" s="15"/>
       <c r="M416" s="15"/>
-      <c r="N416" s="60"/>
+      <c r="N416" s="47"/>
       <c r="O416" s="15"/>
-      <c r="P416" s="60"/>
+      <c r="P416" s="47"/>
       <c r="Q416" s="15"/>
       <c r="R416" s="16"/>
-      <c r="S416" s="63"/>
+      <c r="S416" s="50"/>
       <c r="T416" s="17"/>
     </row>
     <row r="417" spans="6:20" ht="14.25" customHeight="1">
@@ -20450,12 +20451,12 @@
       <c r="K417" s="15"/>
       <c r="L417" s="15"/>
       <c r="M417" s="15"/>
-      <c r="N417" s="60"/>
+      <c r="N417" s="47"/>
       <c r="O417" s="15"/>
-      <c r="P417" s="60"/>
+      <c r="P417" s="47"/>
       <c r="Q417" s="15"/>
       <c r="R417" s="16"/>
-      <c r="S417" s="63"/>
+      <c r="S417" s="50"/>
       <c r="T417" s="17"/>
     </row>
     <row r="418" spans="6:20" ht="14.25" customHeight="1">
@@ -20467,12 +20468,12 @@
       <c r="K418" s="15"/>
       <c r="L418" s="15"/>
       <c r="M418" s="15"/>
-      <c r="N418" s="60"/>
+      <c r="N418" s="47"/>
       <c r="O418" s="15"/>
-      <c r="P418" s="60"/>
+      <c r="P418" s="47"/>
       <c r="Q418" s="15"/>
       <c r="R418" s="16"/>
-      <c r="S418" s="63"/>
+      <c r="S418" s="50"/>
       <c r="T418" s="17"/>
     </row>
     <row r="419" spans="6:20" ht="14.25" customHeight="1">
@@ -20484,12 +20485,12 @@
       <c r="K419" s="15"/>
       <c r="L419" s="15"/>
       <c r="M419" s="15"/>
-      <c r="N419" s="60"/>
+      <c r="N419" s="47"/>
       <c r="O419" s="15"/>
-      <c r="P419" s="60"/>
+      <c r="P419" s="47"/>
       <c r="Q419" s="15"/>
       <c r="R419" s="16"/>
-      <c r="S419" s="63"/>
+      <c r="S419" s="50"/>
       <c r="T419" s="17"/>
     </row>
     <row r="420" spans="6:20" ht="14.25" customHeight="1">
@@ -20501,12 +20502,12 @@
       <c r="K420" s="15"/>
       <c r="L420" s="15"/>
       <c r="M420" s="15"/>
-      <c r="N420" s="60"/>
+      <c r="N420" s="47"/>
       <c r="O420" s="15"/>
-      <c r="P420" s="60"/>
+      <c r="P420" s="47"/>
       <c r="Q420" s="15"/>
       <c r="R420" s="16"/>
-      <c r="S420" s="63"/>
+      <c r="S420" s="50"/>
       <c r="T420" s="17"/>
     </row>
     <row r="421" spans="6:20" ht="14.25" customHeight="1">
@@ -20518,12 +20519,12 @@
       <c r="K421" s="15"/>
       <c r="L421" s="15"/>
       <c r="M421" s="15"/>
-      <c r="N421" s="60"/>
+      <c r="N421" s="47"/>
       <c r="O421" s="15"/>
-      <c r="P421" s="60"/>
+      <c r="P421" s="47"/>
       <c r="Q421" s="15"/>
       <c r="R421" s="16"/>
-      <c r="S421" s="63"/>
+      <c r="S421" s="50"/>
       <c r="T421" s="17"/>
     </row>
     <row r="422" spans="6:20" ht="14.25" customHeight="1">
@@ -20535,12 +20536,12 @@
       <c r="K422" s="15"/>
       <c r="L422" s="15"/>
       <c r="M422" s="15"/>
-      <c r="N422" s="60"/>
+      <c r="N422" s="47"/>
       <c r="O422" s="15"/>
-      <c r="P422" s="60"/>
+      <c r="P422" s="47"/>
       <c r="Q422" s="15"/>
       <c r="R422" s="16"/>
-      <c r="S422" s="63"/>
+      <c r="S422" s="50"/>
       <c r="T422" s="17"/>
     </row>
     <row r="423" spans="6:20" ht="14.25" customHeight="1">
@@ -20552,12 +20553,12 @@
       <c r="K423" s="15"/>
       <c r="L423" s="15"/>
       <c r="M423" s="15"/>
-      <c r="N423" s="60"/>
+      <c r="N423" s="47"/>
       <c r="O423" s="15"/>
-      <c r="P423" s="60"/>
+      <c r="P423" s="47"/>
       <c r="Q423" s="15"/>
       <c r="R423" s="16"/>
-      <c r="S423" s="63"/>
+      <c r="S423" s="50"/>
       <c r="T423" s="17"/>
     </row>
     <row r="424" spans="6:20" ht="14.25" customHeight="1">
@@ -20569,12 +20570,12 @@
       <c r="K424" s="15"/>
       <c r="L424" s="15"/>
       <c r="M424" s="15"/>
-      <c r="N424" s="60"/>
+      <c r="N424" s="47"/>
       <c r="O424" s="15"/>
-      <c r="P424" s="60"/>
+      <c r="P424" s="47"/>
       <c r="Q424" s="15"/>
       <c r="R424" s="16"/>
-      <c r="S424" s="63"/>
+      <c r="S424" s="50"/>
       <c r="T424" s="17"/>
     </row>
     <row r="425" spans="6:20" ht="14.25" customHeight="1">
@@ -20586,12 +20587,12 @@
       <c r="K425" s="15"/>
       <c r="L425" s="15"/>
       <c r="M425" s="15"/>
-      <c r="N425" s="60"/>
+      <c r="N425" s="47"/>
       <c r="O425" s="15"/>
-      <c r="P425" s="60"/>
+      <c r="P425" s="47"/>
       <c r="Q425" s="15"/>
       <c r="R425" s="16"/>
-      <c r="S425" s="63"/>
+      <c r="S425" s="50"/>
       <c r="T425" s="17"/>
     </row>
     <row r="426" spans="6:20" ht="14.25" customHeight="1">
@@ -20603,12 +20604,12 @@
       <c r="K426" s="15"/>
       <c r="L426" s="15"/>
       <c r="M426" s="15"/>
-      <c r="N426" s="60"/>
+      <c r="N426" s="47"/>
       <c r="O426" s="15"/>
-      <c r="P426" s="60"/>
+      <c r="P426" s="47"/>
       <c r="Q426" s="15"/>
       <c r="R426" s="16"/>
-      <c r="S426" s="63"/>
+      <c r="S426" s="50"/>
       <c r="T426" s="17"/>
     </row>
     <row r="427" spans="6:20" ht="14.25" customHeight="1">
@@ -20620,12 +20621,12 @@
       <c r="K427" s="15"/>
       <c r="L427" s="15"/>
       <c r="M427" s="15"/>
-      <c r="N427" s="60"/>
+      <c r="N427" s="47"/>
       <c r="O427" s="15"/>
-      <c r="P427" s="60"/>
+      <c r="P427" s="47"/>
       <c r="Q427" s="15"/>
       <c r="R427" s="16"/>
-      <c r="S427" s="63"/>
+      <c r="S427" s="50"/>
       <c r="T427" s="17"/>
     </row>
     <row r="428" spans="6:20" ht="14.25" customHeight="1">
@@ -20637,12 +20638,12 @@
       <c r="K428" s="15"/>
       <c r="L428" s="15"/>
       <c r="M428" s="15"/>
-      <c r="N428" s="60"/>
+      <c r="N428" s="47"/>
       <c r="O428" s="15"/>
-      <c r="P428" s="60"/>
+      <c r="P428" s="47"/>
       <c r="Q428" s="15"/>
       <c r="R428" s="16"/>
-      <c r="S428" s="63"/>
+      <c r="S428" s="50"/>
       <c r="T428" s="17"/>
     </row>
     <row r="429" spans="6:20" ht="14.25" customHeight="1">
@@ -20654,12 +20655,12 @@
       <c r="K429" s="15"/>
       <c r="L429" s="15"/>
       <c r="M429" s="15"/>
-      <c r="N429" s="60"/>
+      <c r="N429" s="47"/>
       <c r="O429" s="15"/>
-      <c r="P429" s="60"/>
+      <c r="P429" s="47"/>
       <c r="Q429" s="15"/>
       <c r="R429" s="16"/>
-      <c r="S429" s="63"/>
+      <c r="S429" s="50"/>
       <c r="T429" s="17"/>
     </row>
     <row r="430" spans="6:20" ht="14.25" customHeight="1">
@@ -20671,12 +20672,12 @@
       <c r="K430" s="15"/>
       <c r="L430" s="15"/>
       <c r="M430" s="15"/>
-      <c r="N430" s="60"/>
+      <c r="N430" s="47"/>
       <c r="O430" s="15"/>
-      <c r="P430" s="60"/>
+      <c r="P430" s="47"/>
       <c r="Q430" s="15"/>
       <c r="R430" s="16"/>
-      <c r="S430" s="63"/>
+      <c r="S430" s="50"/>
       <c r="T430" s="17"/>
     </row>
     <row r="431" spans="6:20" ht="14.25" customHeight="1">
@@ -20688,12 +20689,12 @@
       <c r="K431" s="15"/>
       <c r="L431" s="15"/>
       <c r="M431" s="15"/>
-      <c r="N431" s="60"/>
+      <c r="N431" s="47"/>
       <c r="O431" s="15"/>
-      <c r="P431" s="60"/>
+      <c r="P431" s="47"/>
       <c r="Q431" s="15"/>
       <c r="R431" s="16"/>
-      <c r="S431" s="63"/>
+      <c r="S431" s="50"/>
       <c r="T431" s="17"/>
     </row>
     <row r="432" spans="6:20" ht="14.25" customHeight="1">
@@ -20705,12 +20706,12 @@
       <c r="K432" s="15"/>
       <c r="L432" s="15"/>
       <c r="M432" s="15"/>
-      <c r="N432" s="60"/>
+      <c r="N432" s="47"/>
       <c r="O432" s="15"/>
-      <c r="P432" s="60"/>
+      <c r="P432" s="47"/>
       <c r="Q432" s="15"/>
       <c r="R432" s="16"/>
-      <c r="S432" s="63"/>
+      <c r="S432" s="50"/>
       <c r="T432" s="17"/>
     </row>
     <row r="433" spans="6:20" ht="14.25" customHeight="1">
@@ -20722,12 +20723,12 @@
       <c r="K433" s="15"/>
       <c r="L433" s="15"/>
       <c r="M433" s="15"/>
-      <c r="N433" s="60"/>
+      <c r="N433" s="47"/>
       <c r="O433" s="15"/>
-      <c r="P433" s="60"/>
+      <c r="P433" s="47"/>
       <c r="Q433" s="15"/>
       <c r="R433" s="16"/>
-      <c r="S433" s="63"/>
+      <c r="S433" s="50"/>
       <c r="T433" s="17"/>
     </row>
     <row r="434" spans="6:20" ht="14.25" customHeight="1">
@@ -20739,12 +20740,12 @@
       <c r="K434" s="15"/>
       <c r="L434" s="15"/>
       <c r="M434" s="15"/>
-      <c r="N434" s="60"/>
+      <c r="N434" s="47"/>
       <c r="O434" s="15"/>
-      <c r="P434" s="60"/>
+      <c r="P434" s="47"/>
       <c r="Q434" s="15"/>
       <c r="R434" s="16"/>
-      <c r="S434" s="63"/>
+      <c r="S434" s="50"/>
       <c r="T434" s="17"/>
     </row>
     <row r="435" spans="6:20" ht="14.25" customHeight="1">
@@ -20756,12 +20757,12 @@
       <c r="K435" s="15"/>
       <c r="L435" s="15"/>
       <c r="M435" s="15"/>
-      <c r="N435" s="60"/>
+      <c r="N435" s="47"/>
       <c r="O435" s="15"/>
-      <c r="P435" s="60"/>
+      <c r="P435" s="47"/>
       <c r="Q435" s="15"/>
       <c r="R435" s="16"/>
-      <c r="S435" s="63"/>
+      <c r="S435" s="50"/>
       <c r="T435" s="17"/>
     </row>
     <row r="436" spans="6:20" ht="14.25" customHeight="1">
@@ -20773,12 +20774,12 @@
       <c r="K436" s="15"/>
       <c r="L436" s="15"/>
       <c r="M436" s="15"/>
-      <c r="N436" s="60"/>
+      <c r="N436" s="47"/>
       <c r="O436" s="15"/>
-      <c r="P436" s="60"/>
+      <c r="P436" s="47"/>
       <c r="Q436" s="15"/>
       <c r="R436" s="16"/>
-      <c r="S436" s="63"/>
+      <c r="S436" s="50"/>
       <c r="T436" s="17"/>
     </row>
     <row r="437" spans="6:20" ht="14.25" customHeight="1">
@@ -20790,12 +20791,12 @@
       <c r="K437" s="15"/>
       <c r="L437" s="15"/>
       <c r="M437" s="15"/>
-      <c r="N437" s="60"/>
+      <c r="N437" s="47"/>
       <c r="O437" s="15"/>
-      <c r="P437" s="60"/>
+      <c r="P437" s="47"/>
       <c r="Q437" s="15"/>
       <c r="R437" s="16"/>
-      <c r="S437" s="63"/>
+      <c r="S437" s="50"/>
       <c r="T437" s="17"/>
     </row>
     <row r="438" spans="6:20" ht="14.25" customHeight="1">
@@ -20807,12 +20808,12 @@
       <c r="K438" s="15"/>
       <c r="L438" s="15"/>
       <c r="M438" s="15"/>
-      <c r="N438" s="60"/>
+      <c r="N438" s="47"/>
       <c r="O438" s="15"/>
-      <c r="P438" s="60"/>
+      <c r="P438" s="47"/>
       <c r="Q438" s="15"/>
       <c r="R438" s="16"/>
-      <c r="S438" s="63"/>
+      <c r="S438" s="50"/>
       <c r="T438" s="17"/>
     </row>
     <row r="439" spans="6:20" ht="14.25" customHeight="1">
@@ -20824,12 +20825,12 @@
       <c r="K439" s="15"/>
       <c r="L439" s="15"/>
       <c r="M439" s="15"/>
-      <c r="N439" s="60"/>
+      <c r="N439" s="47"/>
       <c r="O439" s="15"/>
-      <c r="P439" s="60"/>
+      <c r="P439" s="47"/>
       <c r="Q439" s="15"/>
       <c r="R439" s="16"/>
-      <c r="S439" s="63"/>
+      <c r="S439" s="50"/>
       <c r="T439" s="17"/>
     </row>
     <row r="440" spans="6:20" ht="14.25" customHeight="1">
@@ -20841,12 +20842,12 @@
       <c r="K440" s="15"/>
       <c r="L440" s="15"/>
       <c r="M440" s="15"/>
-      <c r="N440" s="60"/>
+      <c r="N440" s="47"/>
       <c r="O440" s="15"/>
-      <c r="P440" s="60"/>
+      <c r="P440" s="47"/>
       <c r="Q440" s="15"/>
       <c r="R440" s="16"/>
-      <c r="S440" s="63"/>
+      <c r="S440" s="50"/>
       <c r="T440" s="17"/>
     </row>
     <row r="441" spans="6:20" ht="14.25" customHeight="1">
@@ -20858,12 +20859,12 @@
       <c r="K441" s="15"/>
       <c r="L441" s="15"/>
       <c r="M441" s="15"/>
-      <c r="N441" s="60"/>
+      <c r="N441" s="47"/>
       <c r="O441" s="15"/>
-      <c r="P441" s="60"/>
+      <c r="P441" s="47"/>
       <c r="Q441" s="15"/>
       <c r="R441" s="16"/>
-      <c r="S441" s="63"/>
+      <c r="S441" s="50"/>
       <c r="T441" s="17"/>
     </row>
     <row r="442" spans="6:20" ht="14.25" customHeight="1">
@@ -20875,12 +20876,12 @@
       <c r="K442" s="15"/>
       <c r="L442" s="15"/>
       <c r="M442" s="15"/>
-      <c r="N442" s="60"/>
+      <c r="N442" s="47"/>
       <c r="O442" s="15"/>
-      <c r="P442" s="60"/>
+      <c r="P442" s="47"/>
       <c r="Q442" s="15"/>
       <c r="R442" s="16"/>
-      <c r="S442" s="63"/>
+      <c r="S442" s="50"/>
       <c r="T442" s="17"/>
     </row>
     <row r="443" spans="6:20" ht="14.25" customHeight="1">
@@ -20892,12 +20893,12 @@
       <c r="K443" s="15"/>
       <c r="L443" s="15"/>
       <c r="M443" s="15"/>
-      <c r="N443" s="60"/>
+      <c r="N443" s="47"/>
       <c r="O443" s="15"/>
-      <c r="P443" s="60"/>
+      <c r="P443" s="47"/>
       <c r="Q443" s="15"/>
       <c r="R443" s="16"/>
-      <c r="S443" s="63"/>
+      <c r="S443" s="50"/>
       <c r="T443" s="17"/>
     </row>
     <row r="444" spans="6:20" ht="14.25" customHeight="1">
@@ -20909,12 +20910,12 @@
       <c r="K444" s="15"/>
       <c r="L444" s="15"/>
       <c r="M444" s="15"/>
-      <c r="N444" s="60"/>
+      <c r="N444" s="47"/>
       <c r="O444" s="15"/>
-      <c r="P444" s="60"/>
+      <c r="P444" s="47"/>
       <c r="Q444" s="15"/>
       <c r="R444" s="16"/>
-      <c r="S444" s="63"/>
+      <c r="S444" s="50"/>
       <c r="T444" s="17"/>
     </row>
     <row r="445" spans="6:20" ht="14.25" customHeight="1">
@@ -20926,12 +20927,12 @@
       <c r="K445" s="15"/>
       <c r="L445" s="15"/>
       <c r="M445" s="15"/>
-      <c r="N445" s="60"/>
+      <c r="N445" s="47"/>
       <c r="O445" s="15"/>
-      <c r="P445" s="60"/>
+      <c r="P445" s="47"/>
       <c r="Q445" s="15"/>
       <c r="R445" s="16"/>
-      <c r="S445" s="63"/>
+      <c r="S445" s="50"/>
       <c r="T445" s="17"/>
     </row>
     <row r="446" spans="6:20" ht="14.25" customHeight="1">
@@ -20943,12 +20944,12 @@
       <c r="K446" s="15"/>
       <c r="L446" s="15"/>
       <c r="M446" s="15"/>
-      <c r="N446" s="60"/>
+      <c r="N446" s="47"/>
       <c r="O446" s="15"/>
-      <c r="P446" s="60"/>
+      <c r="P446" s="47"/>
       <c r="Q446" s="15"/>
       <c r="R446" s="16"/>
-      <c r="S446" s="63"/>
+      <c r="S446" s="50"/>
       <c r="T446" s="17"/>
     </row>
     <row r="447" spans="6:20" ht="14.25" customHeight="1">
@@ -20960,12 +20961,12 @@
       <c r="K447" s="15"/>
       <c r="L447" s="15"/>
       <c r="M447" s="15"/>
-      <c r="N447" s="60"/>
+      <c r="N447" s="47"/>
       <c r="O447" s="15"/>
-      <c r="P447" s="60"/>
+      <c r="P447" s="47"/>
       <c r="Q447" s="15"/>
       <c r="R447" s="16"/>
-      <c r="S447" s="63"/>
+      <c r="S447" s="50"/>
       <c r="T447" s="17"/>
     </row>
     <row r="448" spans="6:20" ht="14.25" customHeight="1">
@@ -20977,12 +20978,12 @@
       <c r="K448" s="15"/>
       <c r="L448" s="15"/>
       <c r="M448" s="15"/>
-      <c r="N448" s="60"/>
+      <c r="N448" s="47"/>
       <c r="O448" s="15"/>
-      <c r="P448" s="60"/>
+      <c r="P448" s="47"/>
       <c r="Q448" s="15"/>
       <c r="R448" s="16"/>
-      <c r="S448" s="63"/>
+      <c r="S448" s="50"/>
       <c r="T448" s="17"/>
     </row>
     <row r="449" spans="6:20" ht="14.25" customHeight="1">
@@ -20994,12 +20995,12 @@
       <c r="K449" s="15"/>
       <c r="L449" s="15"/>
       <c r="M449" s="15"/>
-      <c r="N449" s="60"/>
+      <c r="N449" s="47"/>
       <c r="O449" s="15"/>
-      <c r="P449" s="60"/>
+      <c r="P449" s="47"/>
       <c r="Q449" s="15"/>
       <c r="R449" s="16"/>
-      <c r="S449" s="63"/>
+      <c r="S449" s="50"/>
       <c r="T449" s="17"/>
     </row>
     <row r="450" spans="6:20" ht="14.25" customHeight="1">
@@ -21011,12 +21012,12 @@
       <c r="K450" s="15"/>
       <c r="L450" s="15"/>
       <c r="M450" s="15"/>
-      <c r="N450" s="60"/>
+      <c r="N450" s="47"/>
       <c r="O450" s="15"/>
-      <c r="P450" s="60"/>
+      <c r="P450" s="47"/>
       <c r="Q450" s="15"/>
       <c r="R450" s="16"/>
-      <c r="S450" s="63"/>
+      <c r="S450" s="50"/>
       <c r="T450" s="17"/>
     </row>
     <row r="451" spans="6:20" ht="14.25" customHeight="1">
@@ -21028,12 +21029,12 @@
       <c r="K451" s="15"/>
       <c r="L451" s="15"/>
       <c r="M451" s="15"/>
-      <c r="N451" s="60"/>
+      <c r="N451" s="47"/>
       <c r="O451" s="15"/>
-      <c r="P451" s="60"/>
+      <c r="P451" s="47"/>
       <c r="Q451" s="15"/>
       <c r="R451" s="16"/>
-      <c r="S451" s="63"/>
+      <c r="S451" s="50"/>
       <c r="T451" s="17"/>
     </row>
     <row r="452" spans="6:20" ht="14.25" customHeight="1">
@@ -21045,12 +21046,12 @@
       <c r="K452" s="15"/>
       <c r="L452" s="15"/>
       <c r="M452" s="15"/>
-      <c r="N452" s="60"/>
+      <c r="N452" s="47"/>
       <c r="O452" s="15"/>
-      <c r="P452" s="60"/>
+      <c r="P452" s="47"/>
       <c r="Q452" s="15"/>
       <c r="R452" s="16"/>
-      <c r="S452" s="63"/>
+      <c r="S452" s="50"/>
       <c r="T452" s="17"/>
     </row>
     <row r="453" spans="6:20" ht="14.25" customHeight="1">
@@ -21062,12 +21063,12 @@
       <c r="K453" s="15"/>
       <c r="L453" s="15"/>
       <c r="M453" s="15"/>
-      <c r="N453" s="60"/>
+      <c r="N453" s="47"/>
       <c r="O453" s="15"/>
-      <c r="P453" s="60"/>
+      <c r="P453" s="47"/>
       <c r="Q453" s="15"/>
       <c r="R453" s="16"/>
-      <c r="S453" s="63"/>
+      <c r="S453" s="50"/>
       <c r="T453" s="17"/>
     </row>
     <row r="454" spans="6:20" ht="14.25" customHeight="1">
@@ -21079,12 +21080,12 @@
       <c r="K454" s="15"/>
       <c r="L454" s="15"/>
       <c r="M454" s="15"/>
-      <c r="N454" s="60"/>
+      <c r="N454" s="47"/>
       <c r="O454" s="15"/>
-      <c r="P454" s="60"/>
+      <c r="P454" s="47"/>
       <c r="Q454" s="15"/>
       <c r="R454" s="16"/>
-      <c r="S454" s="63"/>
+      <c r="S454" s="50"/>
       <c r="T454" s="17"/>
     </row>
     <row r="455" spans="6:20" ht="14.25" customHeight="1">
@@ -21096,12 +21097,12 @@
       <c r="K455" s="15"/>
       <c r="L455" s="15"/>
       <c r="M455" s="15"/>
-      <c r="N455" s="60"/>
+      <c r="N455" s="47"/>
       <c r="O455" s="15"/>
-      <c r="P455" s="60"/>
+      <c r="P455" s="47"/>
       <c r="Q455" s="15"/>
       <c r="R455" s="16"/>
-      <c r="S455" s="63"/>
+      <c r="S455" s="50"/>
       <c r="T455" s="17"/>
     </row>
     <row r="456" spans="6:20" ht="14.25" customHeight="1">
@@ -21113,12 +21114,12 @@
       <c r="K456" s="15"/>
       <c r="L456" s="15"/>
       <c r="M456" s="15"/>
-      <c r="N456" s="60"/>
+      <c r="N456" s="47"/>
       <c r="O456" s="15"/>
-      <c r="P456" s="60"/>
+      <c r="P456" s="47"/>
       <c r="Q456" s="15"/>
       <c r="R456" s="16"/>
-      <c r="S456" s="63"/>
+      <c r="S456" s="50"/>
       <c r="T456" s="17"/>
     </row>
     <row r="457" spans="6:20" ht="14.25" customHeight="1">
@@ -21130,12 +21131,12 @@
       <c r="K457" s="15"/>
       <c r="L457" s="15"/>
       <c r="M457" s="15"/>
-      <c r="N457" s="60"/>
+      <c r="N457" s="47"/>
       <c r="O457" s="15"/>
-      <c r="P457" s="60"/>
+      <c r="P457" s="47"/>
       <c r="Q457" s="15"/>
       <c r="R457" s="16"/>
-      <c r="S457" s="63"/>
+      <c r="S457" s="50"/>
       <c r="T457" s="17"/>
     </row>
     <row r="458" spans="6:20" ht="14.25" customHeight="1">
@@ -21147,12 +21148,12 @@
       <c r="K458" s="15"/>
       <c r="L458" s="15"/>
       <c r="M458" s="15"/>
-      <c r="N458" s="60"/>
+      <c r="N458" s="47"/>
       <c r="O458" s="15"/>
-      <c r="P458" s="60"/>
+      <c r="P458" s="47"/>
       <c r="Q458" s="15"/>
       <c r="R458" s="16"/>
-      <c r="S458" s="63"/>
+      <c r="S458" s="50"/>
       <c r="T458" s="17"/>
     </row>
     <row r="459" spans="6:20" ht="14.25" customHeight="1">
@@ -21164,12 +21165,12 @@
       <c r="K459" s="15"/>
       <c r="L459" s="15"/>
       <c r="M459" s="15"/>
-      <c r="N459" s="60"/>
+      <c r="N459" s="47"/>
       <c r="O459" s="15"/>
-      <c r="P459" s="60"/>
+      <c r="P459" s="47"/>
       <c r="Q459" s="15"/>
       <c r="R459" s="16"/>
-      <c r="S459" s="63"/>
+      <c r="S459" s="50"/>
       <c r="T459" s="17"/>
     </row>
     <row r="460" spans="6:20" ht="14.25" customHeight="1">
@@ -21181,12 +21182,12 @@
       <c r="K460" s="15"/>
       <c r="L460" s="15"/>
       <c r="M460" s="15"/>
-      <c r="N460" s="60"/>
+      <c r="N460" s="47"/>
       <c r="O460" s="15"/>
-      <c r="P460" s="60"/>
+      <c r="P460" s="47"/>
       <c r="Q460" s="15"/>
       <c r="R460" s="16"/>
-      <c r="S460" s="63"/>
+      <c r="S460" s="50"/>
       <c r="T460" s="17"/>
     </row>
     <row r="461" spans="6:20" ht="14.25" customHeight="1">
@@ -21198,12 +21199,12 @@
       <c r="K461" s="15"/>
       <c r="L461" s="15"/>
       <c r="M461" s="15"/>
-      <c r="N461" s="60"/>
+      <c r="N461" s="47"/>
       <c r="O461" s="15"/>
-      <c r="P461" s="60"/>
+      <c r="P461" s="47"/>
       <c r="Q461" s="15"/>
       <c r="R461" s="16"/>
-      <c r="S461" s="63"/>
+      <c r="S461" s="50"/>
       <c r="T461" s="17"/>
     </row>
     <row r="462" spans="6:20" ht="14.25" customHeight="1">
@@ -21215,12 +21216,12 @@
       <c r="K462" s="15"/>
       <c r="L462" s="15"/>
       <c r="M462" s="15"/>
-      <c r="N462" s="60"/>
+      <c r="N462" s="47"/>
       <c r="O462" s="15"/>
-      <c r="P462" s="60"/>
+      <c r="P462" s="47"/>
       <c r="Q462" s="15"/>
       <c r="R462" s="16"/>
-      <c r="S462" s="63"/>
+      <c r="S462" s="50"/>
       <c r="T462" s="17"/>
     </row>
     <row r="463" spans="6:20" ht="14.25" customHeight="1">
@@ -21232,12 +21233,12 @@
       <c r="K463" s="15"/>
       <c r="L463" s="15"/>
       <c r="M463" s="15"/>
-      <c r="N463" s="60"/>
+      <c r="N463" s="47"/>
       <c r="O463" s="15"/>
-      <c r="P463" s="60"/>
+      <c r="P463" s="47"/>
       <c r="Q463" s="15"/>
       <c r="R463" s="16"/>
-      <c r="S463" s="63"/>
+      <c r="S463" s="50"/>
       <c r="T463" s="17"/>
     </row>
     <row r="464" spans="6:20" ht="14.25" customHeight="1">
@@ -21249,12 +21250,12 @@
       <c r="K464" s="15"/>
       <c r="L464" s="15"/>
       <c r="M464" s="15"/>
-      <c r="N464" s="60"/>
+      <c r="N464" s="47"/>
       <c r="O464" s="15"/>
-      <c r="P464" s="60"/>
+      <c r="P464" s="47"/>
       <c r="Q464" s="15"/>
       <c r="R464" s="16"/>
-      <c r="S464" s="63"/>
+      <c r="S464" s="50"/>
       <c r="T464" s="17"/>
     </row>
     <row r="465" spans="6:20" ht="14.25" customHeight="1">
@@ -21266,12 +21267,12 @@
       <c r="K465" s="15"/>
       <c r="L465" s="15"/>
       <c r="M465" s="15"/>
-      <c r="N465" s="60"/>
+      <c r="N465" s="47"/>
       <c r="O465" s="15"/>
-      <c r="P465" s="60"/>
+      <c r="P465" s="47"/>
       <c r="Q465" s="15"/>
       <c r="R465" s="16"/>
-      <c r="S465" s="63"/>
+      <c r="S465" s="50"/>
       <c r="T465" s="17"/>
     </row>
     <row r="466" spans="6:20" ht="14.25" customHeight="1">
@@ -21283,12 +21284,12 @@
       <c r="K466" s="15"/>
       <c r="L466" s="15"/>
       <c r="M466" s="15"/>
-      <c r="N466" s="60"/>
+      <c r="N466" s="47"/>
       <c r="O466" s="15"/>
-      <c r="P466" s="60"/>
+      <c r="P466" s="47"/>
       <c r="Q466" s="15"/>
       <c r="R466" s="16"/>
-      <c r="S466" s="63"/>
+      <c r="S466" s="50"/>
       <c r="T466" s="17"/>
     </row>
     <row r="467" spans="6:20" ht="14.25" customHeight="1">
@@ -21300,12 +21301,12 @@
       <c r="K467" s="15"/>
       <c r="L467" s="15"/>
       <c r="M467" s="15"/>
-      <c r="N467" s="60"/>
+      <c r="N467" s="47"/>
       <c r="O467" s="15"/>
-      <c r="P467" s="60"/>
+      <c r="P467" s="47"/>
       <c r="Q467" s="15"/>
       <c r="R467" s="16"/>
-      <c r="S467" s="63"/>
+      <c r="S467" s="50"/>
       <c r="T467" s="17"/>
     </row>
     <row r="468" spans="6:20" ht="14.25" customHeight="1">
@@ -21317,12 +21318,12 @@
       <c r="K468" s="15"/>
       <c r="L468" s="15"/>
       <c r="M468" s="15"/>
-      <c r="N468" s="60"/>
+      <c r="N468" s="47"/>
       <c r="O468" s="15"/>
-      <c r="P468" s="60"/>
+      <c r="P468" s="47"/>
       <c r="Q468" s="15"/>
       <c r="R468" s="16"/>
-      <c r="S468" s="63"/>
+      <c r="S468" s="50"/>
       <c r="T468" s="17"/>
     </row>
     <row r="469" spans="6:20" ht="14.25" customHeight="1">
@@ -21334,12 +21335,12 @@
       <c r="K469" s="15"/>
       <c r="L469" s="15"/>
       <c r="M469" s="15"/>
-      <c r="N469" s="60"/>
+      <c r="N469" s="47"/>
       <c r="O469" s="15"/>
-      <c r="P469" s="60"/>
+      <c r="P469" s="47"/>
       <c r="Q469" s="15"/>
       <c r="R469" s="16"/>
-      <c r="S469" s="63"/>
+      <c r="S469" s="50"/>
       <c r="T469" s="17"/>
     </row>
     <row r="470" spans="6:20" ht="14.25" customHeight="1">
@@ -21351,12 +21352,12 @@
       <c r="K470" s="15"/>
       <c r="L470" s="15"/>
       <c r="M470" s="15"/>
-      <c r="N470" s="60"/>
+      <c r="N470" s="47"/>
       <c r="O470" s="15"/>
-      <c r="P470" s="60"/>
+      <c r="P470" s="47"/>
       <c r="Q470" s="15"/>
       <c r="R470" s="16"/>
-      <c r="S470" s="63"/>
+      <c r="S470" s="50"/>
       <c r="T470" s="17"/>
     </row>
     <row r="471" spans="6:20" ht="14.25" customHeight="1">
@@ -21368,12 +21369,12 @@
       <c r="K471" s="15"/>
       <c r="L471" s="15"/>
       <c r="M471" s="15"/>
-      <c r="N471" s="60"/>
+      <c r="N471" s="47"/>
       <c r="O471" s="15"/>
-      <c r="P471" s="60"/>
+      <c r="P471" s="47"/>
       <c r="Q471" s="15"/>
       <c r="R471" s="16"/>
-      <c r="S471" s="63"/>
+      <c r="S471" s="50"/>
       <c r="T471" s="17"/>
     </row>
     <row r="472" spans="6:20" ht="14.25" customHeight="1">
@@ -21385,12 +21386,12 @@
       <c r="K472" s="15"/>
       <c r="L472" s="15"/>
       <c r="M472" s="15"/>
-      <c r="N472" s="60"/>
+      <c r="N472" s="47"/>
       <c r="O472" s="15"/>
-      <c r="P472" s="60"/>
+      <c r="P472" s="47"/>
       <c r="Q472" s="15"/>
       <c r="R472" s="16"/>
-      <c r="S472" s="63"/>
+      <c r="S472" s="50"/>
       <c r="T472" s="17"/>
     </row>
     <row r="473" spans="6:20" ht="14.25" customHeight="1">
@@ -21402,12 +21403,12 @@
       <c r="K473" s="15"/>
       <c r="L473" s="15"/>
       <c r="M473" s="15"/>
-      <c r="N473" s="60"/>
+      <c r="N473" s="47"/>
       <c r="O473" s="15"/>
-      <c r="P473" s="60"/>
+      <c r="P473" s="47"/>
       <c r="Q473" s="15"/>
       <c r="R473" s="16"/>
-      <c r="S473" s="63"/>
+      <c r="S473" s="50"/>
       <c r="T473" s="17"/>
     </row>
     <row r="474" spans="6:20" ht="14.25" customHeight="1">
@@ -21419,12 +21420,12 @@
       <c r="K474" s="15"/>
       <c r="L474" s="15"/>
       <c r="M474" s="15"/>
-      <c r="N474" s="60"/>
+      <c r="N474" s="47"/>
       <c r="O474" s="15"/>
-      <c r="P474" s="60"/>
+      <c r="P474" s="47"/>
       <c r="Q474" s="15"/>
       <c r="R474" s="16"/>
-      <c r="S474" s="63"/>
+      <c r="S474" s="50"/>
       <c r="T474" s="17"/>
     </row>
     <row r="475" spans="6:20" ht="14.25" customHeight="1">
@@ -21436,12 +21437,12 @@
       <c r="K475" s="15"/>
       <c r="L475" s="15"/>
       <c r="M475" s="15"/>
-      <c r="N475" s="60"/>
+      <c r="N475" s="47"/>
       <c r="O475" s="15"/>
-      <c r="P475" s="60"/>
+      <c r="P475" s="47"/>
       <c r="Q475" s="15"/>
       <c r="R475" s="16"/>
-      <c r="S475" s="63"/>
+      <c r="S475" s="50"/>
       <c r="T475" s="17"/>
     </row>
     <row r="476" spans="6:20" ht="14.25" customHeight="1">
@@ -21453,12 +21454,12 @@
       <c r="K476" s="15"/>
       <c r="L476" s="15"/>
       <c r="M476" s="15"/>
-      <c r="N476" s="60"/>
+      <c r="N476" s="47"/>
       <c r="O476" s="15"/>
-      <c r="P476" s="60"/>
+      <c r="P476" s="47"/>
       <c r="Q476" s="15"/>
       <c r="R476" s="16"/>
-      <c r="S476" s="63"/>
+      <c r="S476" s="50"/>
       <c r="T476" s="17"/>
     </row>
     <row r="477" spans="6:20" ht="14.25" customHeight="1">
@@ -21470,12 +21471,12 @@
       <c r="K477" s="15"/>
       <c r="L477" s="15"/>
       <c r="M477" s="15"/>
-      <c r="N477" s="60"/>
+      <c r="N477" s="47"/>
       <c r="O477" s="15"/>
-      <c r="P477" s="60"/>
+      <c r="P477" s="47"/>
       <c r="Q477" s="15"/>
       <c r="R477" s="16"/>
-      <c r="S477" s="63"/>
+      <c r="S477" s="50"/>
       <c r="T477" s="17"/>
     </row>
     <row r="478" spans="6:20" ht="14.25" customHeight="1">
@@ -21487,12 +21488,12 @@
       <c r="K478" s="15"/>
       <c r="L478" s="15"/>
       <c r="M478" s="15"/>
-      <c r="N478" s="60"/>
+      <c r="N478" s="47"/>
       <c r="O478" s="15"/>
-      <c r="P478" s="60"/>
+      <c r="P478" s="47"/>
       <c r="Q478" s="15"/>
       <c r="R478" s="16"/>
-      <c r="S478" s="63"/>
+      <c r="S478" s="50"/>
       <c r="T478" s="17"/>
     </row>
     <row r="479" spans="6:20" ht="14.25" customHeight="1">
@@ -21504,12 +21505,12 @@
       <c r="K479" s="15"/>
       <c r="L479" s="15"/>
       <c r="M479" s="15"/>
-      <c r="N479" s="60"/>
+      <c r="N479" s="47"/>
       <c r="O479" s="15"/>
-      <c r="P479" s="60"/>
+      <c r="P479" s="47"/>
       <c r="Q479" s="15"/>
       <c r="R479" s="16"/>
-      <c r="S479" s="63"/>
+      <c r="S479" s="50"/>
       <c r="T479" s="17"/>
     </row>
     <row r="480" spans="6:20" ht="14.25" customHeight="1">
@@ -21521,12 +21522,12 @@
       <c r="K480" s="15"/>
       <c r="L480" s="15"/>
       <c r="M480" s="15"/>
-      <c r="N480" s="60"/>
+      <c r="N480" s="47"/>
       <c r="O480" s="15"/>
-      <c r="P480" s="60"/>
+      <c r="P480" s="47"/>
       <c r="Q480" s="15"/>
       <c r="R480" s="16"/>
-      <c r="S480" s="63"/>
+      <c r="S480" s="50"/>
       <c r="T480" s="17"/>
     </row>
     <row r="481" spans="6:20" ht="14.25" customHeight="1">
@@ -21538,12 +21539,12 @@
       <c r="K481" s="15"/>
       <c r="L481" s="15"/>
       <c r="M481" s="15"/>
-      <c r="N481" s="60"/>
+      <c r="N481" s="47"/>
       <c r="O481" s="15"/>
-      <c r="P481" s="60"/>
+      <c r="P481" s="47"/>
       <c r="Q481" s="15"/>
       <c r="R481" s="16"/>
-      <c r="S481" s="63"/>
+      <c r="S481" s="50"/>
       <c r="T481" s="17"/>
     </row>
     <row r="482" spans="6:20" ht="14.25" customHeight="1">
@@ -21555,12 +21556,12 @@
       <c r="K482" s="15"/>
       <c r="L482" s="15"/>
       <c r="M482" s="15"/>
-      <c r="N482" s="60"/>
+      <c r="N482" s="47"/>
       <c r="O482" s="15"/>
-      <c r="P482" s="60"/>
+      <c r="P482" s="47"/>
       <c r="Q482" s="15"/>
       <c r="R482" s="16"/>
-      <c r="S482" s="63"/>
+      <c r="S482" s="50"/>
       <c r="T482" s="17"/>
     </row>
     <row r="483" spans="6:20" ht="14.25" customHeight="1">
@@ -21572,12 +21573,12 @@
       <c r="K483" s="15"/>
       <c r="L483" s="15"/>
       <c r="M483" s="15"/>
-      <c r="N483" s="60"/>
+      <c r="N483" s="47"/>
       <c r="O483" s="15"/>
-      <c r="P483" s="60"/>
+      <c r="P483" s="47"/>
       <c r="Q483" s="15"/>
       <c r="R483" s="16"/>
-      <c r="S483" s="63"/>
+      <c r="S483" s="50"/>
       <c r="T483" s="17"/>
     </row>
     <row r="484" spans="6:20" ht="14.25" customHeight="1">
@@ -21589,12 +21590,12 @@
       <c r="K484" s="15"/>
       <c r="L484" s="15"/>
       <c r="M484" s="15"/>
-      <c r="N484" s="60"/>
+      <c r="N484" s="47"/>
       <c r="O484" s="15"/>
-      <c r="P484" s="60"/>
+      <c r="P484" s="47"/>
       <c r="Q484" s="15"/>
       <c r="R484" s="16"/>
-      <c r="S484" s="63"/>
+      <c r="S484" s="50"/>
       <c r="T484" s="17"/>
     </row>
     <row r="485" spans="6:20" ht="14.25" customHeight="1">
@@ -21606,12 +21607,12 @@
       <c r="K485" s="15"/>
       <c r="L485" s="15"/>
       <c r="M485" s="15"/>
-      <c r="N485" s="60"/>
+      <c r="N485" s="47"/>
       <c r="O485" s="15"/>
-      <c r="P485" s="60"/>
+      <c r="P485" s="47"/>
       <c r="Q485" s="15"/>
       <c r="R485" s="16"/>
-      <c r="S485" s="63"/>
+      <c r="S485" s="50"/>
       <c r="T485" s="17"/>
     </row>
     <row r="486" spans="6:20" ht="14.25" customHeight="1">
@@ -21623,12 +21624,12 @@
       <c r="K486" s="15"/>
       <c r="L486" s="15"/>
       <c r="M486" s="15"/>
-      <c r="N486" s="60"/>
+      <c r="N486" s="47"/>
       <c r="O486" s="15"/>
-      <c r="P486" s="60"/>
+      <c r="P486" s="47"/>
       <c r="Q486" s="15"/>
       <c r="R486" s="16"/>
-      <c r="S486" s="63"/>
+      <c r="S486" s="50"/>
       <c r="T486" s="17"/>
     </row>
     <row r="487" spans="6:20" ht="14.25" customHeight="1">
@@ -21640,12 +21641,12 @@
       <c r="K487" s="15"/>
       <c r="L487" s="15"/>
       <c r="M487" s="15"/>
-      <c r="N487" s="60"/>
+      <c r="N487" s="47"/>
       <c r="O487" s="15"/>
-      <c r="P487" s="60"/>
+      <c r="P487" s="47"/>
       <c r="Q487" s="15"/>
       <c r="R487" s="16"/>
-      <c r="S487" s="63"/>
+      <c r="S487" s="50"/>
       <c r="T487" s="17"/>
     </row>
     <row r="488" spans="6:20" ht="14.25" customHeight="1">
@@ -21657,12 +21658,12 @@
       <c r="K488" s="15"/>
       <c r="L488" s="15"/>
       <c r="M488" s="15"/>
-      <c r="N488" s="60"/>
+      <c r="N488" s="47"/>
       <c r="O488" s="15"/>
-      <c r="P488" s="60"/>
+      <c r="P488" s="47"/>
       <c r="Q488" s="15"/>
       <c r="R488" s="16"/>
-      <c r="S488" s="63"/>
+      <c r="S488" s="50"/>
       <c r="T488" s="17"/>
     </row>
     <row r="489" spans="6:20" ht="14.25" customHeight="1">
@@ -21674,12 +21675,12 @@
       <c r="K489" s="15"/>
       <c r="L489" s="15"/>
       <c r="M489" s="15"/>
-      <c r="N489" s="60"/>
+      <c r="N489" s="47"/>
       <c r="O489" s="15"/>
-      <c r="P489" s="60"/>
+      <c r="P489" s="47"/>
       <c r="Q489" s="15"/>
       <c r="R489" s="16"/>
-      <c r="S489" s="63"/>
+      <c r="S489" s="50"/>
       <c r="T489" s="17"/>
     </row>
     <row r="490" spans="6:20" ht="14.25" customHeight="1">
@@ -21691,12 +21692,12 @@
       <c r="K490" s="15"/>
       <c r="L490" s="15"/>
       <c r="M490" s="15"/>
-      <c r="N490" s="60"/>
+      <c r="N490" s="47"/>
       <c r="O490" s="15"/>
-      <c r="P490" s="60"/>
+      <c r="P490" s="47"/>
       <c r="Q490" s="15"/>
       <c r="R490" s="16"/>
-      <c r="S490" s="63"/>
+      <c r="S490" s="50"/>
       <c r="T490" s="17"/>
     </row>
     <row r="491" spans="6:20" ht="14.25" customHeight="1">
@@ -21708,12 +21709,12 @@
       <c r="K491" s="15"/>
       <c r="L491" s="15"/>
       <c r="M491" s="15"/>
-      <c r="N491" s="60"/>
+      <c r="N491" s="47"/>
       <c r="O491" s="15"/>
-      <c r="P491" s="60"/>
+      <c r="P491" s="47"/>
       <c r="Q491" s="15"/>
       <c r="R491" s="16"/>
-      <c r="S491" s="63"/>
+      <c r="S491" s="50"/>
       <c r="T491" s="17"/>
     </row>
     <row r="492" spans="6:20" ht="14.25" customHeight="1">
@@ -21725,12 +21726,12 @@
       <c r="K492" s="15"/>
       <c r="L492" s="15"/>
       <c r="M492" s="15"/>
-      <c r="N492" s="60"/>
+      <c r="N492" s="47"/>
       <c r="O492" s="15"/>
-      <c r="P492" s="60"/>
+      <c r="P492" s="47"/>
       <c r="Q492" s="15"/>
       <c r="R492" s="16"/>
-      <c r="S492" s="63"/>
+      <c r="S492" s="50"/>
       <c r="T492" s="17"/>
     </row>
     <row r="493" spans="6:20" ht="14.25" customHeight="1">
@@ -21742,12 +21743,12 @@
       <c r="K493" s="15"/>
       <c r="L493" s="15"/>
       <c r="M493" s="15"/>
-      <c r="N493" s="60"/>
+      <c r="N493" s="47"/>
       <c r="O493" s="15"/>
-      <c r="P493" s="60"/>
+      <c r="P493" s="47"/>
       <c r="Q493" s="15"/>
       <c r="R493" s="16"/>
-      <c r="S493" s="63"/>
+      <c r="S493" s="50"/>
       <c r="T493" s="17"/>
     </row>
     <row r="494" spans="6:20" ht="14.25" customHeight="1">
@@ -21759,12 +21760,12 @@
       <c r="K494" s="15"/>
       <c r="L494" s="15"/>
       <c r="M494" s="15"/>
-      <c r="N494" s="60"/>
+      <c r="N494" s="47"/>
       <c r="O494" s="15"/>
-      <c r="P494" s="60"/>
+      <c r="P494" s="47"/>
       <c r="Q494" s="15"/>
       <c r="R494" s="16"/>
-      <c r="S494" s="63"/>
+      <c r="S494" s="50"/>
       <c r="T494" s="17"/>
     </row>
     <row r="495" spans="6:20" ht="14.25" customHeight="1">
@@ -21776,12 +21777,12 @@
       <c r="K495" s="15"/>
       <c r="L495" s="15"/>
       <c r="M495" s="15"/>
-      <c r="N495" s="60"/>
+      <c r="N495" s="47"/>
       <c r="O495" s="15"/>
-      <c r="P495" s="60"/>
+      <c r="P495" s="47"/>
       <c r="Q495" s="15"/>
       <c r="R495" s="16"/>
-      <c r="S495" s="63"/>
+      <c r="S495" s="50"/>
       <c r="T495" s="17"/>
     </row>
     <row r="496" spans="6:20" ht="14.25" customHeight="1">
@@ -21793,12 +21794,12 @@
       <c r="K496" s="15"/>
       <c r="L496" s="15"/>
       <c r="M496" s="15"/>
-      <c r="N496" s="60"/>
+      <c r="N496" s="47"/>
       <c r="O496" s="15"/>
-      <c r="P496" s="60"/>
+      <c r="P496" s="47"/>
       <c r="Q496" s="15"/>
       <c r="R496" s="16"/>
-      <c r="S496" s="63"/>
+      <c r="S496" s="50"/>
       <c r="T496" s="17"/>
     </row>
     <row r="497" spans="6:20" ht="14.25" customHeight="1">
@@ -21810,12 +21811,12 @@
       <c r="K497" s="15"/>
       <c r="L497" s="15"/>
       <c r="M497" s="15"/>
-      <c r="N497" s="60"/>
+      <c r="N497" s="47"/>
       <c r="O497" s="15"/>
-      <c r="P497" s="60"/>
+      <c r="P497" s="47"/>
       <c r="Q497" s="15"/>
       <c r="R497" s="16"/>
-      <c r="S497" s="63"/>
+      <c r="S497" s="50"/>
       <c r="T497" s="17"/>
     </row>
     <row r="498" spans="6:20" ht="14.25" customHeight="1">
@@ -21827,12 +21828,12 @@
       <c r="K498" s="15"/>
       <c r="L498" s="15"/>
       <c r="M498" s="15"/>
-      <c r="N498" s="60"/>
+      <c r="N498" s="47"/>
       <c r="O498" s="15"/>
-      <c r="P498" s="60"/>
+      <c r="P498" s="47"/>
       <c r="Q498" s="15"/>
       <c r="R498" s="16"/>
-      <c r="S498" s="63"/>
+      <c r="S498" s="50"/>
       <c r="T498" s="17"/>
     </row>
     <row r="499" spans="6:20" ht="14.25" customHeight="1">
@@ -21844,12 +21845,12 @@
       <c r="K499" s="15"/>
       <c r="L499" s="15"/>
       <c r="M499" s="15"/>
-      <c r="N499" s="60"/>
+      <c r="N499" s="47"/>
       <c r="O499" s="15"/>
-      <c r="P499" s="60"/>
+      <c r="P499" s="47"/>
       <c r="Q499" s="15"/>
       <c r="R499" s="16"/>
-      <c r="S499" s="63"/>
+      <c r="S499" s="50"/>
       <c r="T499" s="17"/>
     </row>
     <row r="500" spans="6:20" ht="14.25" customHeight="1">
@@ -21861,12 +21862,12 @@
       <c r="K500" s="15"/>
       <c r="L500" s="15"/>
       <c r="M500" s="15"/>
-      <c r="N500" s="60"/>
+      <c r="N500" s="47"/>
       <c r="O500" s="15"/>
-      <c r="P500" s="60"/>
+      <c r="P500" s="47"/>
       <c r="Q500" s="15"/>
       <c r="R500" s="16"/>
-      <c r="S500" s="63"/>
+      <c r="S500" s="50"/>
       <c r="T500" s="17"/>
     </row>
     <row r="501" spans="6:20" ht="14.25" customHeight="1">
@@ -21878,12 +21879,12 @@
       <c r="K501" s="15"/>
       <c r="L501" s="15"/>
       <c r="M501" s="15"/>
-      <c r="N501" s="60"/>
+      <c r="N501" s="47"/>
       <c r="O501" s="15"/>
-      <c r="P501" s="60"/>
+      <c r="P501" s="47"/>
       <c r="Q501" s="15"/>
       <c r="R501" s="16"/>
-      <c r="S501" s="63"/>
+      <c r="S501" s="50"/>
       <c r="T501" s="17"/>
     </row>
     <row r="502" spans="6:20" ht="14.25" customHeight="1">
@@ -21895,12 +21896,12 @@
       <c r="K502" s="15"/>
       <c r="L502" s="15"/>
       <c r="M502" s="15"/>
-      <c r="N502" s="60"/>
+      <c r="N502" s="47"/>
       <c r="O502" s="15"/>
-      <c r="P502" s="60"/>
+      <c r="P502" s="47"/>
       <c r="Q502" s="15"/>
       <c r="R502" s="16"/>
-      <c r="S502" s="63"/>
+      <c r="S502" s="50"/>
       <c r="T502" s="17"/>
     </row>
     <row r="503" spans="6:20" ht="14.25" customHeight="1">
@@ -21912,12 +21913,12 @@
       <c r="K503" s="15"/>
       <c r="L503" s="15"/>
       <c r="M503" s="15"/>
-      <c r="N503" s="60"/>
+      <c r="N503" s="47"/>
       <c r="O503" s="15"/>
-      <c r="P503" s="60"/>
+      <c r="P503" s="47"/>
       <c r="Q503" s="15"/>
       <c r="R503" s="16"/>
-      <c r="S503" s="63"/>
+      <c r="S503" s="50"/>
       <c r="T503" s="17"/>
     </row>
     <row r="504" spans="6:20" ht="14.25" customHeight="1">
@@ -21929,12 +21930,12 @@
       <c r="K504" s="15"/>
       <c r="L504" s="15"/>
       <c r="M504" s="15"/>
-      <c r="N504" s="60"/>
+      <c r="N504" s="47"/>
       <c r="O504" s="15"/>
-      <c r="P504" s="60"/>
+      <c r="P504" s="47"/>
       <c r="Q504" s="15"/>
       <c r="R504" s="16"/>
-      <c r="S504" s="63"/>
+      <c r="S504" s="50"/>
       <c r="T504" s="17"/>
     </row>
     <row r="505" spans="6:20" ht="14.25" customHeight="1">
@@ -21946,12 +21947,12 @@
       <c r="K505" s="15"/>
       <c r="L505" s="15"/>
       <c r="M505" s="15"/>
-      <c r="N505" s="60"/>
+      <c r="N505" s="47"/>
       <c r="O505" s="15"/>
-      <c r="P505" s="60"/>
+      <c r="P505" s="47"/>
       <c r="Q505" s="15"/>
       <c r="R505" s="16"/>
-      <c r="S505" s="63"/>
+      <c r="S505" s="50"/>
       <c r="T505" s="17"/>
     </row>
     <row r="506" spans="6:20" ht="14.25" customHeight="1">
@@ -21963,12 +21964,12 @@
       <c r="K506" s="15"/>
       <c r="L506" s="15"/>
       <c r="M506" s="15"/>
-      <c r="N506" s="60"/>
+      <c r="N506" s="47"/>
       <c r="O506" s="15"/>
-      <c r="P506" s="60"/>
+      <c r="P506" s="47"/>
       <c r="Q506" s="15"/>
       <c r="R506" s="16"/>
-      <c r="S506" s="63"/>
+      <c r="S506" s="50"/>
       <c r="T506" s="17"/>
     </row>
     <row r="507" spans="6:20" ht="14.25" customHeight="1">
@@ -21980,12 +21981,12 @@
       <c r="K507" s="15"/>
       <c r="L507" s="15"/>
       <c r="M507" s="15"/>
-      <c r="N507" s="60"/>
+      <c r="N507" s="47"/>
       <c r="O507" s="15"/>
-      <c r="P507" s="60"/>
+      <c r="P507" s="47"/>
       <c r="Q507" s="15"/>
       <c r="R507" s="16"/>
-      <c r="S507" s="63"/>
+      <c r="S507" s="50"/>
       <c r="T507" s="17"/>
     </row>
     <row r="508" spans="6:20" ht="14.25" customHeight="1">
@@ -21997,12 +21998,12 @@
       <c r="K508" s="15"/>
       <c r="L508" s="15"/>
       <c r="M508" s="15"/>
-      <c r="N508" s="60"/>
+      <c r="N508" s="47"/>
       <c r="O508" s="15"/>
-      <c r="P508" s="60"/>
+      <c r="P508" s="47"/>
       <c r="Q508" s="15"/>
       <c r="R508" s="16"/>
-      <c r="S508" s="63"/>
+      <c r="S508" s="50"/>
       <c r="T508" s="17"/>
     </row>
     <row r="509" spans="6:20" ht="14.25" customHeight="1">
@@ -22014,12 +22015,12 @@
       <c r="K509" s="15"/>
       <c r="L509" s="15"/>
       <c r="M509" s="15"/>
-      <c r="N509" s="60"/>
+      <c r="N509" s="47"/>
       <c r="O509" s="15"/>
-      <c r="P509" s="60"/>
+      <c r="P509" s="47"/>
       <c r="Q509" s="15"/>
       <c r="R509" s="16"/>
-      <c r="S509" s="63"/>
+      <c r="S509" s="50"/>
       <c r="T509" s="17"/>
     </row>
     <row r="510" spans="6:20" ht="14.25" customHeight="1">
@@ -22031,12 +22032,12 @@
       <c r="K510" s="15"/>
       <c r="L510" s="15"/>
       <c r="M510" s="15"/>
-      <c r="N510" s="60"/>
+      <c r="N510" s="47"/>
       <c r="O510" s="15"/>
-      <c r="P510" s="60"/>
+      <c r="P510" s="47"/>
       <c r="Q510" s="15"/>
       <c r="R510" s="16"/>
-      <c r="S510" s="63"/>
+      <c r="S510" s="50"/>
       <c r="T510" s="17"/>
     </row>
     <row r="511" spans="6:20" ht="14.25" customHeight="1">
@@ -22048,12 +22049,12 @@
       <c r="K511" s="15"/>
       <c r="L511" s="15"/>
       <c r="M511" s="15"/>
-      <c r="N511" s="60"/>
+      <c r="N511" s="47"/>
       <c r="O511" s="15"/>
-      <c r="P511" s="60"/>
+      <c r="P511" s="47"/>
       <c r="Q511" s="15"/>
       <c r="R511" s="16"/>
-      <c r="S511" s="63"/>
+      <c r="S511" s="50"/>
       <c r="T511" s="17"/>
     </row>
     <row r="512" spans="6:20" ht="14.25" customHeight="1">
@@ -22065,12 +22066,12 @@
       <c r="K512" s="15"/>
       <c r="L512" s="15"/>
       <c r="M512" s="15"/>
-      <c r="N512" s="60"/>
+      <c r="N512" s="47"/>
       <c r="O512" s="15"/>
-      <c r="P512" s="60"/>
+      <c r="P512" s="47"/>
       <c r="Q512" s="15"/>
       <c r="R512" s="16"/>
-      <c r="S512" s="63"/>
+      <c r="S512" s="50"/>
       <c r="T512" s="17"/>
     </row>
     <row r="513" spans="6:20" ht="14.25" customHeight="1">
@@ -22082,12 +22083,12 @@
       <c r="K513" s="15"/>
       <c r="L513" s="15"/>
       <c r="M513" s="15"/>
-      <c r="N513" s="60"/>
+      <c r="N513" s="47"/>
       <c r="O513" s="15"/>
-      <c r="P513" s="60"/>
+      <c r="P513" s="47"/>
       <c r="Q513" s="15"/>
       <c r="R513" s="16"/>
-      <c r="S513" s="63"/>
+      <c r="S513" s="50"/>
       <c r="T513" s="17"/>
     </row>
     <row r="514" spans="6:20" ht="14.25" customHeight="1">
@@ -22099,12 +22100,12 @@
       <c r="K514" s="15"/>
       <c r="L514" s="15"/>
       <c r="M514" s="15"/>
-      <c r="N514" s="60"/>
+      <c r="N514" s="47"/>
       <c r="O514" s="15"/>
-      <c r="P514" s="60"/>
+      <c r="P514" s="47"/>
       <c r="Q514" s="15"/>
       <c r="R514" s="16"/>
-      <c r="S514" s="63"/>
+      <c r="S514" s="50"/>
       <c r="T514" s="17"/>
     </row>
     <row r="515" spans="6:20" ht="14.25" customHeight="1">
@@ -22116,12 +22117,12 @@
       <c r="K515" s="15"/>
       <c r="L515" s="15"/>
       <c r="M515" s="15"/>
-      <c r="N515" s="60"/>
+      <c r="N515" s="47"/>
       <c r="O515" s="15"/>
-      <c r="P515" s="60"/>
+      <c r="P515" s="47"/>
       <c r="Q515" s="15"/>
       <c r="R515" s="16"/>
-      <c r="S515" s="63"/>
+      <c r="S515" s="50"/>
       <c r="T515" s="17"/>
     </row>
     <row r="516" spans="6:20" ht="14.25" customHeight="1">
@@ -22133,12 +22134,12 @@
       <c r="K516" s="15"/>
       <c r="L516" s="15"/>
       <c r="M516" s="15"/>
-      <c r="N516" s="60"/>
+      <c r="N516" s="47"/>
       <c r="O516" s="15"/>
-      <c r="P516" s="60"/>
+      <c r="P516" s="47"/>
       <c r="Q516" s="15"/>
       <c r="R516" s="16"/>
-      <c r="S516" s="63"/>
+      <c r="S516" s="50"/>
       <c r="T516" s="17"/>
     </row>
     <row r="517" spans="6:20" ht="14.25" customHeight="1">
@@ -22150,12 +22151,12 @@
       <c r="K517" s="15"/>
       <c r="L517" s="15"/>
       <c r="M517" s="15"/>
-      <c r="N517" s="60"/>
+      <c r="N517" s="47"/>
       <c r="O517" s="15"/>
-      <c r="P517" s="60"/>
+      <c r="P517" s="47"/>
       <c r="Q517" s="15"/>
       <c r="R517" s="16"/>
-      <c r="S517" s="63"/>
+      <c r="S517" s="50"/>
       <c r="T517" s="17"/>
     </row>
     <row r="518" spans="6:20" ht="14.25" customHeight="1">
@@ -22167,12 +22168,12 @@
       <c r="K518" s="15"/>
       <c r="L518" s="15"/>
       <c r="M518" s="15"/>
-      <c r="N518" s="60"/>
+      <c r="N518" s="47"/>
       <c r="O518" s="15"/>
-      <c r="P518" s="60"/>
+      <c r="P518" s="47"/>
       <c r="Q518" s="15"/>
       <c r="R518" s="16"/>
-      <c r="S518" s="63"/>
+      <c r="S518" s="50"/>
       <c r="T518" s="17"/>
     </row>
     <row r="519" spans="6:20" ht="14.25" customHeight="1">
@@ -22184,12 +22185,12 @@
       <c r="K519" s="15"/>
       <c r="L519" s="15"/>
       <c r="M519" s="15"/>
-      <c r="N519" s="60"/>
+      <c r="N519" s="47"/>
       <c r="O519" s="15"/>
-      <c r="P519" s="60"/>
+      <c r="P519" s="47"/>
       <c r="Q519" s="15"/>
       <c r="R519" s="16"/>
-      <c r="S519" s="63"/>
+      <c r="S519" s="50"/>
       <c r="T519" s="17"/>
     </row>
     <row r="520" spans="6:20" ht="14.25" customHeight="1">
@@ -22201,12 +22202,12 @@
       <c r="K520" s="15"/>
       <c r="L520" s="15"/>
       <c r="M520" s="15"/>
-      <c r="N520" s="60"/>
+      <c r="N520" s="47"/>
       <c r="O520" s="15"/>
-      <c r="P520" s="60"/>
+      <c r="P520" s="47"/>
       <c r="Q520" s="15"/>
       <c r="R520" s="16"/>
-      <c r="S520" s="63"/>
+      <c r="S520" s="50"/>
       <c r="T520" s="17"/>
     </row>
     <row r="521" spans="6:20" ht="14.25" customHeight="1">
@@ -22218,12 +22219,12 @@
       <c r="K521" s="15"/>
       <c r="L521" s="15"/>
       <c r="M521" s="15"/>
-      <c r="N521" s="60"/>
+      <c r="N521" s="47"/>
       <c r="O521" s="15"/>
-      <c r="P521" s="60"/>
+      <c r="P521" s="47"/>
       <c r="Q521" s="15"/>
       <c r="R521" s="16"/>
-      <c r="S521" s="63"/>
+      <c r="S521" s="50"/>
       <c r="T521" s="17"/>
     </row>
     <row r="522" spans="6:20" ht="14.25" customHeight="1">
@@ -22235,12 +22236,12 @@
       <c r="K522" s="15"/>
       <c r="L522" s="15"/>
       <c r="M522" s="15"/>
-      <c r="N522" s="60"/>
+      <c r="N522" s="47"/>
       <c r="O522" s="15"/>
-      <c r="P522" s="60"/>
+      <c r="P522" s="47"/>
       <c r="Q522" s="15"/>
       <c r="R522" s="16"/>
-      <c r="S522" s="63"/>
+      <c r="S522" s="50"/>
       <c r="T522" s="17"/>
     </row>
     <row r="523" spans="6:20" ht="14.25" customHeight="1">
@@ -22252,12 +22253,12 @@
       <c r="K523" s="15"/>
       <c r="L523" s="15"/>
       <c r="M523" s="15"/>
-      <c r="N523" s="60"/>
+      <c r="N523" s="47"/>
       <c r="O523" s="15"/>
-      <c r="P523" s="60"/>
+      <c r="P523" s="47"/>
       <c r="Q523" s="15"/>
       <c r="R523" s="16"/>
-      <c r="S523" s="63"/>
+      <c r="S523" s="50"/>
       <c r="T523" s="17"/>
     </row>
     <row r="524" spans="6:20" ht="14.25" customHeight="1">
@@ -22269,12 +22270,12 @@
       <c r="K524" s="15"/>
       <c r="L524" s="15"/>
       <c r="M524" s="15"/>
-      <c r="N524" s="60"/>
+      <c r="N524" s="47"/>
       <c r="O524" s="15"/>
-      <c r="P524" s="60"/>
+      <c r="P524" s="47"/>
       <c r="Q524" s="15"/>
       <c r="R524" s="16"/>
-      <c r="S524" s="63"/>
+      <c r="S524" s="50"/>
       <c r="T524" s="17"/>
     </row>
     <row r="525" spans="6:20" ht="14.25" customHeight="1">
@@ -22286,12 +22287,12 @@
       <c r="K525" s="15"/>
       <c r="L525" s="15"/>
       <c r="M525" s="15"/>
-      <c r="N525" s="60"/>
+      <c r="N525" s="47"/>
       <c r="O525" s="15"/>
-      <c r="P525" s="60"/>
+      <c r="P525" s="47"/>
       <c r="Q525" s="15"/>
       <c r="R525" s="16"/>
-      <c r="S525" s="63"/>
+      <c r="S525" s="50"/>
       <c r="T525" s="17"/>
     </row>
     <row r="526" spans="6:20" ht="14.25" customHeight="1">
@@ -22303,12 +22304,12 @@
       <c r="K526" s="15"/>
       <c r="L526" s="15"/>
       <c r="M526" s="15"/>
-      <c r="N526" s="60"/>
+      <c r="N526" s="47"/>
       <c r="O526" s="15"/>
-      <c r="P526" s="60"/>
+      <c r="P526" s="47"/>
       <c r="Q526" s="15"/>
       <c r="R526" s="16"/>
-      <c r="S526" s="63"/>
+      <c r="S526" s="50"/>
       <c r="T526" s="17"/>
     </row>
     <row r="527" spans="6:20" ht="14.25" customHeight="1">
@@ -22320,12 +22321,12 @@
       <c r="K527" s="15"/>
       <c r="L527" s="15"/>
       <c r="M527" s="15"/>
-      <c r="N527" s="60"/>
+      <c r="N527" s="47"/>
       <c r="O527" s="15"/>
-      <c r="P527" s="60"/>
+      <c r="P527" s="47"/>
       <c r="Q527" s="15"/>
       <c r="R527" s="16"/>
-      <c r="S527" s="63"/>
+      <c r="S527" s="50"/>
       <c r="T527" s="17"/>
     </row>
     <row r="528" spans="6:20" ht="14.25" customHeight="1">
@@ -22337,12 +22338,12 @@
       <c r="K528" s="15"/>
       <c r="L528" s="15"/>
       <c r="M528" s="15"/>
-      <c r="N528" s="60"/>
+      <c r="N528" s="47"/>
       <c r="O528" s="15"/>
-      <c r="P528" s="60"/>
+      <c r="P528" s="47"/>
       <c r="Q528" s="15"/>
       <c r="R528" s="16"/>
-      <c r="S528" s="63"/>
+      <c r="S528" s="50"/>
       <c r="T528" s="17"/>
     </row>
     <row r="529" spans="6:20" ht="14.25" customHeight="1">
@@ -22354,12 +22355,12 @@
       <c r="K529" s="15"/>
       <c r="L529" s="15"/>
       <c r="M529" s="15"/>
-      <c r="N529" s="60"/>
+      <c r="N529" s="47"/>
       <c r="O529" s="15"/>
-      <c r="P529" s="60"/>
+      <c r="P529" s="47"/>
       <c r="Q529" s="15"/>
       <c r="R529" s="16"/>
-      <c r="S529" s="63"/>
+      <c r="S529" s="50"/>
       <c r="T529" s="17"/>
     </row>
     <row r="530" spans="6:20" ht="14.25" customHeight="1">
@@ -22371,12 +22372,12 @@
       <c r="K530" s="15"/>
       <c r="L530" s="15"/>
       <c r="M530" s="15"/>
-      <c r="N530" s="60"/>
+      <c r="N530" s="47"/>
       <c r="O530" s="15"/>
-      <c r="P530" s="60"/>
+      <c r="P530" s="47"/>
       <c r="Q530" s="15"/>
       <c r="R530" s="16"/>
-      <c r="S530" s="63"/>
+      <c r="S530" s="50"/>
       <c r="T530" s="17"/>
     </row>
     <row r="531" spans="6:20" ht="14.25" customHeight="1">
@@ -22388,12 +22389,12 @@
       <c r="K531" s="15"/>
       <c r="L531" s="15"/>
       <c r="M531" s="15"/>
-      <c r="N531" s="60"/>
+      <c r="N531" s="47"/>
       <c r="O531" s="15"/>
-      <c r="P531" s="60"/>
+      <c r="P531" s="47"/>
       <c r="Q531" s="15"/>
       <c r="R531" s="16"/>
-      <c r="S531" s="63"/>
+      <c r="S531" s="50"/>
       <c r="T531" s="17"/>
     </row>
     <row r="532" spans="6:20" ht="14.25" customHeight="1">
@@ -22405,12 +22406,12 @@
       <c r="K532" s="15"/>
       <c r="L532" s="15"/>
       <c r="M532" s="15"/>
-      <c r="N532" s="60"/>
+      <c r="N532" s="47"/>
       <c r="O532" s="15"/>
-      <c r="P532" s="60"/>
+      <c r="P532" s="47"/>
       <c r="Q532" s="15"/>
       <c r="R532" s="16"/>
-      <c r="S532" s="63"/>
+      <c r="S532" s="50"/>
       <c r="T532" s="17"/>
     </row>
     <row r="533" spans="6:20" ht="14.25" customHeight="1">
@@ -22422,12 +22423,12 @@
       <c r="K533" s="15"/>
       <c r="L533" s="15"/>
       <c r="M533" s="15"/>
-      <c r="N533" s="60"/>
+      <c r="N533" s="47"/>
       <c r="O533" s="15"/>
-      <c r="P533" s="60"/>
+      <c r="P533" s="47"/>
       <c r="Q533" s="15"/>
       <c r="R533" s="16"/>
-      <c r="S533" s="63"/>
+      <c r="S533" s="50"/>
       <c r="T533" s="17"/>
     </row>
     <row r="534" spans="6:20" ht="14.25" customHeight="1">
@@ -22439,12 +22440,12 @@
       <c r="K534" s="15"/>
       <c r="L534" s="15"/>
       <c r="M534" s="15"/>
-      <c r="N534" s="60"/>
+      <c r="N534" s="47"/>
       <c r="O534" s="15"/>
-      <c r="P534" s="60"/>
+      <c r="P534" s="47"/>
       <c r="Q534" s="15"/>
       <c r="R534" s="16"/>
-      <c r="S534" s="63"/>
+      <c r="S534" s="50"/>
       <c r="T534" s="17"/>
     </row>
     <row r="535" spans="6:20" ht="14.25" customHeight="1">
@@ -22456,12 +22457,12 @@
       <c r="K535" s="15"/>
       <c r="L535" s="15"/>
       <c r="M535" s="15"/>
-      <c r="N535" s="60"/>
+      <c r="N535" s="47"/>
       <c r="O535" s="15"/>
-      <c r="P535" s="60"/>
+      <c r="P535" s="47"/>
       <c r="Q535" s="15"/>
       <c r="R535" s="16"/>
-      <c r="S535" s="63"/>
+      <c r="S535" s="50"/>
       <c r="T535" s="17"/>
     </row>
     <row r="536" spans="6:20" ht="14.25" customHeight="1">
@@ -22473,12 +22474,12 @@
       <c r="K536" s="15"/>
       <c r="L536" s="15"/>
       <c r="M536" s="15"/>
-      <c r="N536" s="60"/>
+      <c r="N536" s="47"/>
       <c r="O536" s="15"/>
-      <c r="P536" s="60"/>
+      <c r="P536" s="47"/>
       <c r="Q536" s="15"/>
       <c r="R536" s="16"/>
-      <c r="S536" s="63"/>
+      <c r="S536" s="50"/>
       <c r="T536" s="17"/>
     </row>
     <row r="537" spans="6:20" ht="14.25" customHeight="1">
@@ -22490,12 +22491,12 @@
       <c r="K537" s="15"/>
       <c r="L537" s="15"/>
       <c r="M537" s="15"/>
-      <c r="N537" s="60"/>
+      <c r="N537" s="47"/>
       <c r="O537" s="15"/>
-      <c r="P537" s="60"/>
+      <c r="P537" s="47"/>
       <c r="Q537" s="15"/>
       <c r="R537" s="16"/>
-      <c r="S537" s="63"/>
+      <c r="S537" s="50"/>
       <c r="T537" s="17"/>
     </row>
     <row r="538" spans="6:20" ht="14.25" customHeight="1">
@@ -22507,12 +22508,12 @@
       <c r="K538" s="15"/>
       <c r="L538" s="15"/>
       <c r="M538" s="15"/>
-      <c r="N538" s="60"/>
+      <c r="N538" s="47"/>
       <c r="O538" s="15"/>
-      <c r="P538" s="60"/>
+      <c r="P538" s="47"/>
       <c r="Q538" s="15"/>
       <c r="R538" s="16"/>
-      <c r="S538" s="63"/>
+      <c r="S538" s="50"/>
       <c r="T538" s="17"/>
     </row>
     <row r="539" spans="6:20" ht="14.25" customHeight="1">
@@ -22524,12 +22525,12 @@
       <c r="K539" s="15"/>
       <c r="L539" s="15"/>
       <c r="M539" s="15"/>
-      <c r="N539" s="60"/>
+      <c r="N539" s="47"/>
       <c r="O539" s="15"/>
-      <c r="P539" s="60"/>
+      <c r="P539" s="47"/>
       <c r="Q539" s="15"/>
       <c r="R539" s="16"/>
-      <c r="S539" s="63"/>
+      <c r="S539" s="50"/>
       <c r="T539" s="17"/>
     </row>
     <row r="540" spans="6:20" ht="14.25" customHeight="1">
@@ -22541,12 +22542,12 @@
       <c r="K540" s="15"/>
       <c r="L540" s="15"/>
       <c r="M540" s="15"/>
-      <c r="N540" s="60"/>
+      <c r="N540" s="47"/>
       <c r="O540" s="15"/>
-      <c r="P540" s="60"/>
+      <c r="P540" s="47"/>
       <c r="Q540" s="15"/>
       <c r="R540" s="16"/>
-      <c r="S540" s="63"/>
+      <c r="S540" s="50"/>
       <c r="T540" s="17"/>
     </row>
     <row r="541" spans="6:20" ht="14.25" customHeight="1">
@@ -22558,12 +22559,12 @@
       <c r="K541" s="15"/>
       <c r="L541" s="15"/>
       <c r="M541" s="15"/>
-      <c r="N541" s="60"/>
+      <c r="N541" s="47"/>
       <c r="O541" s="15"/>
-      <c r="P541" s="60"/>
+      <c r="P541" s="47"/>
       <c r="Q541" s="15"/>
       <c r="R541" s="16"/>
-      <c r="S541" s="63"/>
+      <c r="S541" s="50"/>
       <c r="T541" s="17"/>
     </row>
     <row r="542" spans="6:20" ht="14.25" customHeight="1">
@@ -22575,12 +22576,12 @@
       <c r="K542" s="15"/>
       <c r="L542" s="15"/>
       <c r="M542" s="15"/>
-      <c r="N542" s="60"/>
+      <c r="N542" s="47"/>
       <c r="O542" s="15"/>
-      <c r="P542" s="60"/>
+      <c r="P542" s="47"/>
       <c r="Q542" s="15"/>
       <c r="R542" s="16"/>
-      <c r="S542" s="63"/>
+      <c r="S542" s="50"/>
       <c r="T542" s="17"/>
     </row>
     <row r="543" spans="6:20" ht="14.25" customHeight="1">
@@ -22592,12 +22593,12 @@
       <c r="K543" s="15"/>
       <c r="L543" s="15"/>
       <c r="M543" s="15"/>
-      <c r="N543" s="60"/>
+      <c r="N543" s="47"/>
       <c r="O543" s="15"/>
-      <c r="P543" s="60"/>
+      <c r="P543" s="47"/>
       <c r="Q543" s="15"/>
       <c r="R543" s="16"/>
-      <c r="S543" s="63"/>
+      <c r="S543" s="50"/>
       <c r="T543" s="17"/>
     </row>
     <row r="544" spans="6:20" ht="14.25" customHeight="1">
@@ -22609,12 +22610,12 @@
       <c r="K544" s="15"/>
       <c r="L544" s="15"/>
       <c r="M544" s="15"/>
-      <c r="N544" s="60"/>
+      <c r="N544" s="47"/>
       <c r="O544" s="15"/>
-      <c r="P544" s="60"/>
+      <c r="P544" s="47"/>
       <c r="Q544" s="15"/>
       <c r="R544" s="16"/>
-      <c r="S544" s="63"/>
+      <c r="S544" s="50"/>
       <c r="T544" s="17"/>
     </row>
     <row r="545" spans="6:20" ht="14.25" customHeight="1">
@@ -22626,12 +22627,12 @@
       <c r="K545" s="15"/>
       <c r="L545" s="15"/>
       <c r="M545" s="15"/>
-      <c r="N545" s="60"/>
+      <c r="N545" s="47"/>
       <c r="O545" s="15"/>
-      <c r="P545" s="60"/>
+      <c r="P545" s="47"/>
       <c r="Q545" s="15"/>
       <c r="R545" s="16"/>
-      <c r="S545" s="63"/>
+      <c r="S545" s="50"/>
       <c r="T545" s="17"/>
     </row>
     <row r="546" spans="6:20" ht="14.25" customHeight="1">
@@ -22643,12 +22644,12 @@
       <c r="K546" s="15"/>
       <c r="L546" s="15"/>
       <c r="M546" s="15"/>
-      <c r="N546" s="60"/>
+      <c r="N546" s="47"/>
       <c r="O546" s="15"/>
-      <c r="P546" s="60"/>
+      <c r="P546" s="47"/>
       <c r="Q546" s="15"/>
       <c r="R546" s="16"/>
-      <c r="S546" s="63"/>
+      <c r="S546" s="50"/>
       <c r="T546" s="17"/>
     </row>
     <row r="547" spans="6:20" ht="14.25" customHeight="1">
@@ -22660,12 +22661,12 @@
       <c r="K547" s="15"/>
       <c r="L547" s="15"/>
       <c r="M547" s="15"/>
-      <c r="N547" s="60"/>
+      <c r="N547" s="47"/>
       <c r="O547" s="15"/>
-      <c r="P547" s="60"/>
+      <c r="P547" s="47"/>
       <c r="Q547" s="15"/>
       <c r="R547" s="16"/>
-      <c r="S547" s="63"/>
+      <c r="S547" s="50"/>
       <c r="T547" s="17"/>
     </row>
     <row r="548" spans="6:20" ht="14.25" customHeight="1">
@@ -22677,12 +22678,12 @@
       <c r="K548" s="15"/>
       <c r="L548" s="15"/>
       <c r="M548" s="15"/>
-      <c r="N548" s="60"/>
+      <c r="N548" s="47"/>
       <c r="O548" s="15"/>
-      <c r="P548" s="60"/>
+      <c r="P548" s="47"/>
       <c r="Q548" s="15"/>
       <c r="R548" s="16"/>
-      <c r="S548" s="63"/>
+      <c r="S548" s="50"/>
       <c r="T548" s="17"/>
     </row>
     <row r="549" spans="6:20" ht="14.25" customHeight="1">
@@ -22694,12 +22695,12 @@
       <c r="K549" s="15"/>
       <c r="L549" s="15"/>
       <c r="M549" s="15"/>
-      <c r="N549" s="60"/>
+      <c r="N549" s="47"/>
       <c r="O549" s="15"/>
-      <c r="P549" s="60"/>
+      <c r="P549" s="47"/>
       <c r="Q549" s="15"/>
       <c r="R549" s="16"/>
-      <c r="S549" s="63"/>
+      <c r="S549" s="50"/>
       <c r="T549" s="17"/>
     </row>
     <row r="550" spans="6:20" ht="14.25" customHeight="1">
@@ -22711,12 +22712,12 @@
       <c r="K550" s="15"/>
       <c r="L550" s="15"/>
       <c r="M550" s="15"/>
-      <c r="N550" s="60"/>
+      <c r="N550" s="47"/>
       <c r="O550" s="15"/>
-      <c r="P550" s="60"/>
+      <c r="P550" s="47"/>
       <c r="Q550" s="15"/>
       <c r="R550" s="16"/>
-      <c r="S550" s="63"/>
+      <c r="S550" s="50"/>
       <c r="T550" s="17"/>
     </row>
     <row r="551" spans="6:20" ht="14.25" customHeight="1">
@@ -22728,12 +22729,12 @@
       <c r="K551" s="15"/>
       <c r="L551" s="15"/>
       <c r="M551" s="15"/>
-      <c r="N551" s="60"/>
+      <c r="N551" s="47"/>
       <c r="O551" s="15"/>
-      <c r="P551" s="60"/>
+      <c r="P551" s="47"/>
       <c r="Q551" s="15"/>
       <c r="R551" s="16"/>
-      <c r="S551" s="63"/>
+      <c r="S551" s="50"/>
       <c r="T551" s="17"/>
     </row>
     <row r="552" spans="6:20" ht="14.25" customHeight="1">
@@ -22745,12 +22746,12 @@
       <c r="K552" s="15"/>
       <c r="L552" s="15"/>
       <c r="M552" s="15"/>
-      <c r="N552" s="60"/>
+      <c r="N552" s="47"/>
       <c r="O552" s="15"/>
-      <c r="P552" s="60"/>
+      <c r="P552" s="47"/>
       <c r="Q552" s="15"/>
       <c r="R552" s="16"/>
-      <c r="S552" s="63"/>
+      <c r="S552" s="50"/>
       <c r="T552" s="17"/>
     </row>
     <row r="553" spans="6:20" ht="14.25" customHeight="1">
@@ -22762,12 +22763,12 @@
       <c r="K553" s="15"/>
       <c r="L553" s="15"/>
       <c r="M553" s="15"/>
-      <c r="N553" s="60"/>
+      <c r="N553" s="47"/>
       <c r="O553" s="15"/>
-      <c r="P553" s="60"/>
+      <c r="P553" s="47"/>
       <c r="Q553" s="15"/>
       <c r="R553" s="16"/>
-      <c r="S553" s="63"/>
+      <c r="S553" s="50"/>
       <c r="T553" s="17"/>
     </row>
     <row r="554" spans="6:20" ht="14.25" customHeight="1">
@@ -22779,12 +22780,12 @@
       <c r="K554" s="15"/>
       <c r="L554" s="15"/>
       <c r="M554" s="15"/>
-      <c r="N554" s="60"/>
+      <c r="N554" s="47"/>
       <c r="O554" s="15"/>
-      <c r="P554" s="60"/>
+      <c r="P554" s="47"/>
       <c r="Q554" s="15"/>
       <c r="R554" s="16"/>
-      <c r="S554" s="63"/>
+      <c r="S554" s="50"/>
       <c r="T554" s="17"/>
     </row>
     <row r="555" spans="6:20" ht="14.25" customHeight="1">
@@ -22796,12 +22797,12 @@
       <c r="K555" s="15"/>
       <c r="L555" s="15"/>
       <c r="M555" s="15"/>
-      <c r="N555" s="60"/>
+      <c r="N555" s="47"/>
       <c r="O555" s="15"/>
-      <c r="P555" s="60"/>
+      <c r="P555" s="47"/>
       <c r="Q555" s="15"/>
       <c r="R555" s="16"/>
-      <c r="S555" s="63"/>
+      <c r="S555" s="50"/>
       <c r="T555" s="17"/>
     </row>
     <row r="556" spans="6:20" ht="14.25" customHeight="1">
@@ -22813,12 +22814,12 @@
       <c r="K556" s="15"/>
       <c r="L556" s="15"/>
       <c r="M556" s="15"/>
-      <c r="N556" s="60"/>
+      <c r="N556" s="47"/>
       <c r="O556" s="15"/>
-      <c r="P556" s="60"/>
+      <c r="P556" s="47"/>
       <c r="Q556" s="15"/>
       <c r="R556" s="16"/>
-      <c r="S556" s="63"/>
+      <c r="S556" s="50"/>
       <c r="T556" s="17"/>
     </row>
     <row r="557" spans="6:20" ht="14.25" customHeight="1">
@@ -22830,12 +22831,12 @@
       <c r="K557" s="15"/>
       <c r="L557" s="15"/>
       <c r="M557" s="15"/>
-      <c r="N557" s="60"/>
+      <c r="N557" s="47"/>
       <c r="O557" s="15"/>
-      <c r="P557" s="60"/>
+      <c r="P557" s="47"/>
       <c r="Q557" s="15"/>
       <c r="R557" s="16"/>
-      <c r="S557" s="63"/>
+      <c r="S557" s="50"/>
       <c r="T557" s="17"/>
     </row>
     <row r="558" spans="6:20" ht="14.25" customHeight="1">
@@ -22847,12 +22848,12 @@
       <c r="K558" s="15"/>
       <c r="L558" s="15"/>
       <c r="M558" s="15"/>
-      <c r="N558" s="60"/>
+      <c r="N558" s="47"/>
       <c r="O558" s="15"/>
-      <c r="P558" s="60"/>
+      <c r="P558" s="47"/>
       <c r="Q558" s="15"/>
       <c r="R558" s="16"/>
-      <c r="S558" s="63"/>
+      <c r="S558" s="50"/>
       <c r="T558" s="17"/>
     </row>
     <row r="559" spans="6:20" ht="14.25" customHeight="1">
@@ -22864,12 +22865,12 @@
       <c r="K559" s="15"/>
       <c r="L559" s="15"/>
       <c r="M559" s="15"/>
-      <c r="N559" s="60"/>
+      <c r="N559" s="47"/>
       <c r="O559" s="15"/>
-      <c r="P559" s="60"/>
+      <c r="P559" s="47"/>
       <c r="Q559" s="15"/>
       <c r="R559" s="16"/>
-      <c r="S559" s="63"/>
+      <c r="S559" s="50"/>
       <c r="T559" s="17"/>
     </row>
     <row r="560" spans="6:20" ht="14.25" customHeight="1">
@@ -22881,12 +22882,12 @@
       <c r="K560" s="15"/>
       <c r="L560" s="15"/>
       <c r="M560" s="15"/>
-      <c r="N560" s="60"/>
+      <c r="N560" s="47"/>
       <c r="O560" s="15"/>
-      <c r="P560" s="60"/>
+      <c r="P560" s="47"/>
       <c r="Q560" s="15"/>
       <c r="R560" s="16"/>
-      <c r="S560" s="63"/>
+      <c r="S560" s="50"/>
       <c r="T560" s="17"/>
     </row>
     <row r="561" spans="6:20" ht="14.25" customHeight="1">
@@ -22898,12 +22899,12 @@
       <c r="K561" s="15"/>
       <c r="L561" s="15"/>
       <c r="M561" s="15"/>
-      <c r="N561" s="60"/>
+      <c r="N561" s="47"/>
       <c r="O561" s="15"/>
-      <c r="P561" s="60"/>
+      <c r="P561" s="47"/>
       <c r="Q561" s="15"/>
       <c r="R561" s="16"/>
-      <c r="S561" s="63"/>
+      <c r="S561" s="50"/>
       <c r="T561" s="17"/>
     </row>
     <row r="562" spans="6:20" ht="14.25" customHeight="1">
@@ -22915,12 +22916,12 @@
       <c r="K562" s="15"/>
       <c r="L562" s="15"/>
       <c r="M562" s="15"/>
-      <c r="N562" s="60"/>
+      <c r="N562" s="47"/>
       <c r="O562" s="15"/>
-      <c r="P562" s="60"/>
+      <c r="P562" s="47"/>
       <c r="Q562" s="15"/>
       <c r="R562" s="16"/>
-      <c r="S562" s="63"/>
+      <c r="S562" s="50"/>
       <c r="T562" s="17"/>
     </row>
     <row r="563" spans="6:20" ht="14.25" customHeight="1">
@@ -22932,12 +22933,12 @@
       <c r="K563" s="15"/>
       <c r="L563" s="15"/>
       <c r="M563" s="15"/>
-      <c r="N563" s="60"/>
+      <c r="N563" s="47"/>
       <c r="O563" s="15"/>
-      <c r="P563" s="60"/>
+      <c r="P563" s="47"/>
       <c r="Q563" s="15"/>
       <c r="R563" s="16"/>
-      <c r="S563" s="63"/>
+      <c r="S563" s="50"/>
       <c r="T563" s="17"/>
     </row>
     <row r="564" spans="6:20" ht="14.25" customHeight="1">
@@ -22949,12 +22950,12 @@
       <c r="K564" s="15"/>
       <c r="L564" s="15"/>
       <c r="M564" s="15"/>
-      <c r="N564" s="60"/>
+      <c r="N564" s="47"/>
       <c r="O564" s="15"/>
-      <c r="P564" s="60"/>
+      <c r="P564" s="47"/>
       <c r="Q564" s="15"/>
       <c r="R564" s="16"/>
-      <c r="S564" s="63"/>
+      <c r="S564" s="50"/>
       <c r="T564" s="17"/>
     </row>
     <row r="565" spans="6:20" ht="14.25" customHeight="1">
@@ -22966,12 +22967,12 @@
       <c r="K565" s="15"/>
       <c r="L565" s="15"/>
       <c r="M565" s="15"/>
-      <c r="N565" s="60"/>
+      <c r="N565" s="47"/>
       <c r="O565" s="15"/>
-      <c r="P565" s="60"/>
+      <c r="P565" s="47"/>
       <c r="Q565" s="15"/>
       <c r="R565" s="16"/>
-      <c r="S565" s="63"/>
+      <c r="S565" s="50"/>
       <c r="T565" s="17"/>
     </row>
     <row r="566" spans="6:20" ht="14.25" customHeight="1">
@@ -22983,12 +22984,12 @@
       <c r="K566" s="15"/>
       <c r="L566" s="15"/>
       <c r="M566" s="15"/>
-      <c r="N566" s="60"/>
+      <c r="N566" s="47"/>
       <c r="O566" s="15"/>
-      <c r="P566" s="60"/>
+      <c r="P566" s="47"/>
       <c r="Q566" s="15"/>
       <c r="R566" s="16"/>
-      <c r="S566" s="63"/>
+      <c r="S566" s="50"/>
       <c r="T566" s="17"/>
     </row>
     <row r="567" spans="6:20" ht="14.25" customHeight="1">
@@ -23000,12 +23001,12 @@
       <c r="K567" s="15"/>
       <c r="L567" s="15"/>
       <c r="M567" s="15"/>
-      <c r="N567" s="60"/>
+      <c r="N567" s="47"/>
       <c r="O567" s="15"/>
-      <c r="P567" s="60"/>
+      <c r="P567" s="47"/>
       <c r="Q567" s="15"/>
       <c r="R567" s="16"/>
-      <c r="S567" s="63"/>
+      <c r="S567" s="50"/>
       <c r="T567" s="17"/>
     </row>
     <row r="568" spans="6:20" ht="14.25" customHeight="1">
@@ -23017,12 +23018,12 @@
       <c r="K568" s="15"/>
       <c r="L568" s="15"/>
       <c r="M568" s="15"/>
-      <c r="N568" s="60"/>
+      <c r="N568" s="47"/>
       <c r="O568" s="15"/>
-      <c r="P568" s="60"/>
+      <c r="P568" s="47"/>
       <c r="Q568" s="15"/>
       <c r="R568" s="16"/>
-      <c r="S568" s="63"/>
+      <c r="S568" s="50"/>
       <c r="T568" s="17"/>
     </row>
     <row r="569" spans="6:20" ht="14.25" customHeight="1">
@@ -23034,12 +23035,12 @@
       <c r="K569" s="15"/>
       <c r="L569" s="15"/>
       <c r="M569" s="15"/>
-      <c r="N569" s="60"/>
+      <c r="N569" s="47"/>
       <c r="O569" s="15"/>
-      <c r="P569" s="60"/>
+      <c r="P569" s="47"/>
       <c r="Q569" s="15"/>
       <c r="R569" s="16"/>
-      <c r="S569" s="63"/>
+      <c r="S569" s="50"/>
       <c r="T569" s="17"/>
     </row>
     <row r="570" spans="6:20" ht="14.25" customHeight="1">
@@ -23051,12 +23052,12 @@
       <c r="K570" s="15"/>
       <c r="L570" s="15"/>
       <c r="M570" s="15"/>
-      <c r="N570" s="60"/>
+      <c r="N570" s="47"/>
       <c r="O570" s="15"/>
-      <c r="P570" s="60"/>
+      <c r="P570" s="47"/>
       <c r="Q570" s="15"/>
       <c r="R570" s="16"/>
-      <c r="S570" s="63"/>
+      <c r="S570" s="50"/>
       <c r="T570" s="17"/>
     </row>
     <row r="571" spans="6:20" ht="14.25" customHeight="1">
@@ -23068,12 +23069,12 @@
       <c r="K571" s="15"/>
       <c r="L571" s="15"/>
       <c r="M571" s="15"/>
-      <c r="N571" s="60"/>
+      <c r="N571" s="47"/>
       <c r="O571" s="15"/>
-      <c r="P571" s="60"/>
+      <c r="P571" s="47"/>
       <c r="Q571" s="15"/>
       <c r="R571" s="16"/>
-      <c r="S571" s="63"/>
+      <c r="S571" s="50"/>
       <c r="T571" s="17"/>
     </row>
     <row r="572" spans="6:20" ht="14.25" customHeight="1">
@@ -23085,12 +23086,12 @@
       <c r="K572" s="15"/>
       <c r="L572" s="15"/>
       <c r="M572" s="15"/>
-      <c r="N572" s="60"/>
+      <c r="N572" s="47"/>
       <c r="O572" s="15"/>
-      <c r="P572" s="60"/>
+      <c r="P572" s="47"/>
       <c r="Q572" s="15"/>
       <c r="R572" s="16"/>
-      <c r="S572" s="63"/>
+      <c r="S572" s="50"/>
       <c r="T572" s="17"/>
     </row>
     <row r="573" spans="6:20" ht="14.25" customHeight="1">
@@ -23102,12 +23103,12 @@
       <c r="K573" s="15"/>
       <c r="L573" s="15"/>
       <c r="M573" s="15"/>
-      <c r="N573" s="60"/>
+      <c r="N573" s="47"/>
       <c r="O573" s="15"/>
-      <c r="P573" s="60"/>
+      <c r="P573" s="47"/>
       <c r="Q573" s="15"/>
       <c r="R573" s="16"/>
-      <c r="S573" s="63"/>
+      <c r="S573" s="50"/>
       <c r="T573" s="17"/>
     </row>
     <row r="574" spans="6:20" ht="14.25" customHeight="1">
@@ -23119,12 +23120,12 @@
       <c r="K574" s="15"/>
       <c r="L574" s="15"/>
       <c r="M574" s="15"/>
-      <c r="N574" s="60"/>
+      <c r="N574" s="47"/>
       <c r="O574" s="15"/>
-      <c r="P574" s="60"/>
+      <c r="P574" s="47"/>
       <c r="Q574" s="15"/>
       <c r="R574" s="16"/>
-      <c r="S574" s="63"/>
+      <c r="S574" s="50"/>
       <c r="T574" s="17"/>
     </row>
     <row r="575" spans="6:20" ht="14.25" customHeight="1">
@@ -23136,12 +23137,12 @@
       <c r="K575" s="15"/>
       <c r="L575" s="15"/>
       <c r="M575" s="15"/>
-      <c r="N575" s="60"/>
+      <c r="N575" s="47"/>
       <c r="O575" s="15"/>
-      <c r="P575" s="60"/>
+      <c r="P575" s="47"/>
       <c r="Q575" s="15"/>
       <c r="R575" s="16"/>
-      <c r="S575" s="63"/>
+      <c r="S575" s="50"/>
       <c r="T575" s="17"/>
     </row>
     <row r="576" spans="6:20" ht="14.25" customHeight="1">
@@ -23153,12 +23154,12 @@
       <c r="K576" s="15"/>
       <c r="L576" s="15"/>
       <c r="M576" s="15"/>
-      <c r="N576" s="60"/>
+      <c r="N576" s="47"/>
       <c r="O576" s="15"/>
-      <c r="P576" s="60"/>
+      <c r="P576" s="47"/>
       <c r="Q576" s="15"/>
       <c r="R576" s="16"/>
-      <c r="S576" s="63"/>
+      <c r="S576" s="50"/>
       <c r="T576" s="17"/>
     </row>
     <row r="577" spans="6:20" ht="14.25" customHeight="1">
@@ -23170,12 +23171,12 @@
       <c r="K577" s="15"/>
       <c r="L577" s="15"/>
       <c r="M577" s="15"/>
-      <c r="N577" s="60"/>
+      <c r="N577" s="47"/>
       <c r="O577" s="15"/>
-      <c r="P577" s="60"/>
+      <c r="P577" s="47"/>
       <c r="Q577" s="15"/>
       <c r="R577" s="16"/>
-      <c r="S577" s="63"/>
+      <c r="S577" s="50"/>
       <c r="T577" s="17"/>
     </row>
     <row r="578" spans="6:20" ht="14.25" customHeight="1">
@@ -23187,12 +23188,12 @@
       <c r="K578" s="15"/>
       <c r="L578" s="15"/>
       <c r="M578" s="15"/>
-      <c r="N578" s="60"/>
+      <c r="N578" s="47"/>
       <c r="O578" s="15"/>
-      <c r="P578" s="60"/>
+      <c r="P578" s="47"/>
       <c r="Q578" s="15"/>
       <c r="R578" s="16"/>
-      <c r="S578" s="63"/>
+      <c r="S578" s="50"/>
       <c r="T578" s="17"/>
     </row>
     <row r="579" spans="6:20" ht="14.25" customHeight="1">
@@ -23204,12 +23205,12 @@
       <c r="K579" s="15"/>
       <c r="L579" s="15"/>
       <c r="M579" s="15"/>
-      <c r="N579" s="60"/>
+      <c r="N579" s="47"/>
       <c r="O579" s="15"/>
-      <c r="P579" s="60"/>
+      <c r="P579" s="47"/>
       <c r="Q579" s="15"/>
       <c r="R579" s="16"/>
-      <c r="S579" s="63"/>
+      <c r="S579" s="50"/>
       <c r="T579" s="17"/>
     </row>
     <row r="580" spans="6:20" ht="14.25" customHeight="1">
@@ -23221,12 +23222,12 @@
       <c r="K580" s="15"/>
       <c r="L580" s="15"/>
       <c r="M580" s="15"/>
-      <c r="N580" s="60"/>
+      <c r="N580" s="47"/>
       <c r="O580" s="15"/>
-      <c r="P580" s="60"/>
+      <c r="P580" s="47"/>
       <c r="Q580" s="15"/>
       <c r="R580" s="16"/>
-      <c r="S580" s="63"/>
+      <c r="S580" s="50"/>
       <c r="T580" s="17"/>
     </row>
     <row r="581" spans="6:20" ht="14.25" customHeight="1">
@@ -23238,12 +23239,12 @@
       <c r="K581" s="15"/>
       <c r="L581" s="15"/>
       <c r="M581" s="15"/>
-      <c r="N581" s="60"/>
+      <c r="N581" s="47"/>
       <c r="O581" s="15"/>
-      <c r="P581" s="60"/>
+      <c r="P581" s="47"/>
       <c r="Q581" s="15"/>
       <c r="R581" s="16"/>
-      <c r="S581" s="63"/>
+      <c r="S581" s="50"/>
       <c r="T581" s="17"/>
     </row>
     <row r="582" spans="6:20" ht="14.25" customHeight="1">
@@ -23255,12 +23256,12 @@
       <c r="K582" s="15"/>
       <c r="L582" s="15"/>
       <c r="M582" s="15"/>
-      <c r="N582" s="60"/>
+      <c r="N582" s="47"/>
       <c r="O582" s="15"/>
-      <c r="P582" s="60"/>
+      <c r="P582" s="47"/>
       <c r="Q582" s="15"/>
       <c r="R582" s="16"/>
-      <c r="S582" s="63"/>
+      <c r="S582" s="50"/>
       <c r="T582" s="17"/>
     </row>
     <row r="583" spans="6:20" ht="14.25" customHeight="1">
@@ -23272,12 +23273,12 @@
       <c r="K583" s="15"/>
       <c r="L583" s="15"/>
       <c r="M583" s="15"/>
-      <c r="N583" s="60"/>
+      <c r="N583" s="47"/>
       <c r="O583" s="15"/>
-      <c r="P583" s="60"/>
+      <c r="P583" s="47"/>
       <c r="Q583" s="15"/>
       <c r="R583" s="16"/>
-      <c r="S583" s="63"/>
+      <c r="S583" s="50"/>
       <c r="T583" s="17"/>
     </row>
     <row r="584" spans="6:20" ht="14.25" customHeight="1">
@@ -24532,7 +24533,7 @@
       <c r="T1000" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T383">
+  <autoFilter ref="A9:T383" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
@@ -24560,13 +24561,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>O163:O198 O382:O383 O10:O36 J10:J198 L38:M38 O38 L40:M44 O40:O44 L54:M198 L46:M46 L375:M383 L48:M52 O48:O52 J381 M47 J231:J246 J295:J310 J335:J338 J351:J354 J363:J364 J371:J372 J377 O56:O82 O84 O87:O153 O155:O158 O160 O375:O376 O378:O380 L10:M36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -24579,7 +24580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D1000"/>
   <sheetViews>
@@ -24598,16 +24599,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="40" t="s">
         <v>844</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>845</v>
       </c>
     </row>
@@ -24618,10 +24619,10 @@
       <c r="B2" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="41" t="s">
         <v>847</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>848</v>
       </c>
     </row>
@@ -24632,24 +24633,24 @@
       <c r="B3" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="41" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>846</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="43" t="s">
         <v>851</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="44" t="s">
         <v>852</v>
       </c>
     </row>
@@ -24660,10 +24661,10 @@
       <c r="B5" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>853</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>854</v>
       </c>
     </row>
@@ -24674,10 +24675,10 @@
       <c r="B6" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>855</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="45" t="s">
         <v>856</v>
       </c>
     </row>
@@ -24688,24 +24689,24 @@
       <c r="B7" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>857</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="45" t="s">
         <v>858</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>846</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>859</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="44" t="s">
         <v>860</v>
       </c>
     </row>
@@ -24716,10 +24717,10 @@
       <c r="B9" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="41" t="s">
         <v>861</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="45" t="s">
         <v>862</v>
       </c>
     </row>
@@ -24730,10 +24731,10 @@
       <c r="B10" s="13" t="s">
         <v>846</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="45" t="s">
         <v>864</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>865</v>
       </c>
     </row>
@@ -24744,10 +24745,10 @@
       <c r="B11" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="41">
         <v>192</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="41" t="s">
         <v>867</v>
       </c>
     </row>
@@ -24758,10 +24759,10 @@
       <c r="B12" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="41">
         <v>208</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>868</v>
       </c>
     </row>
@@ -24772,10 +24773,10 @@
       <c r="B13" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="41">
         <v>224</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="45" t="s">
         <v>869</v>
       </c>
     </row>
@@ -24786,10 +24787,10 @@
       <c r="B14" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="41">
         <v>240</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>870</v>
       </c>
     </row>
@@ -24800,10 +24801,10 @@
       <c r="B15" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="41">
         <v>256</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="45" t="s">
         <v>871</v>
       </c>
     </row>
@@ -24814,10 +24815,10 @@
       <c r="B16" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="41">
         <v>272</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="45" t="s">
         <v>872</v>
       </c>
     </row>
@@ -24828,10 +24829,10 @@
       <c r="B17" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="41">
         <v>288</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="45" t="s">
         <v>873</v>
       </c>
     </row>
@@ -24842,10 +24843,10 @@
       <c r="B18" s="13" t="s">
         <v>866</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="41">
         <v>304</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>874</v>
       </c>
     </row>
@@ -24856,10 +24857,10 @@
       <c r="B19" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <v>193</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="41" t="s">
         <v>876</v>
       </c>
     </row>
@@ -24870,10 +24871,10 @@
       <c r="B20" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="41">
         <v>209</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="41" t="s">
         <v>877</v>
       </c>
     </row>
@@ -24884,10 +24885,10 @@
       <c r="B21" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="41">
         <v>225</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="45" t="s">
         <v>878</v>
       </c>
     </row>
@@ -24898,10 +24899,10 @@
       <c r="B22" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="41">
         <v>241</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="41" t="s">
         <v>879</v>
       </c>
     </row>
@@ -24912,10 +24913,10 @@
       <c r="B23" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="41">
         <v>257</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="45" t="s">
         <v>880</v>
       </c>
     </row>
@@ -24926,10 +24927,10 @@
       <c r="B24" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="41">
         <v>273</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="45" t="s">
         <v>881</v>
       </c>
     </row>
@@ -24940,10 +24941,10 @@
       <c r="B25" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="41">
         <v>289</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="45" t="s">
         <v>882</v>
       </c>
     </row>
@@ -24954,10 +24955,10 @@
       <c r="B26" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="41">
         <v>305</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="45" t="s">
         <v>883</v>
       </c>
     </row>
@@ -24968,10 +24969,10 @@
       <c r="B27" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="41">
         <v>194</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="41" t="s">
         <v>885</v>
       </c>
     </row>
@@ -24982,10 +24983,10 @@
       <c r="B28" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C28" s="42">
+      <c r="C28" s="41">
         <v>210</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="41" t="s">
         <v>886</v>
       </c>
     </row>
@@ -24996,10 +24997,10 @@
       <c r="B29" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C29" s="42">
+      <c r="C29" s="41">
         <v>226</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="46" t="s">
         <v>887</v>
       </c>
     </row>
@@ -25010,10 +25011,10 @@
       <c r="B30" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="41">
         <v>242</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="41" t="s">
         <v>888</v>
       </c>
     </row>
@@ -25024,10 +25025,10 @@
       <c r="B31" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="41">
         <v>258</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="45" t="s">
         <v>889</v>
       </c>
     </row>
@@ -25038,10 +25039,10 @@
       <c r="B32" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="41">
         <v>274</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="45" t="s">
         <v>890</v>
       </c>
     </row>
@@ -25052,10 +25053,10 @@
       <c r="B33" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="41">
         <v>290</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="45" t="s">
         <v>891</v>
       </c>
     </row>
@@ -25066,10 +25067,10 @@
       <c r="B34" s="13" t="s">
         <v>884</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="41">
         <v>306</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="45" t="s">
         <v>892</v>
       </c>
     </row>
@@ -25080,10 +25081,10 @@
       <c r="B35" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="41">
         <v>195</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="41">
         <v>204</v>
       </c>
     </row>
@@ -25094,10 +25095,10 @@
       <c r="B36" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C36" s="42">
+      <c r="C36" s="41">
         <v>211</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="41">
         <v>220</v>
       </c>
     </row>
@@ -25108,10 +25109,10 @@
       <c r="B37" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C37" s="42">
+      <c r="C37" s="41">
         <v>227</v>
       </c>
-      <c r="D37" s="46">
+      <c r="D37" s="45">
         <v>236</v>
       </c>
     </row>
@@ -25122,10 +25123,10 @@
       <c r="B38" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C38" s="42">
+      <c r="C38" s="41">
         <v>243</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="41">
         <v>252</v>
       </c>
     </row>
@@ -25136,10 +25137,10 @@
       <c r="B39" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C39" s="42">
+      <c r="C39" s="41">
         <v>259</v>
       </c>
-      <c r="D39" s="46">
+      <c r="D39" s="45">
         <v>268</v>
       </c>
     </row>
@@ -25150,10 +25151,10 @@
       <c r="B40" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C40" s="42">
+      <c r="C40" s="41">
         <v>275</v>
       </c>
-      <c r="D40" s="46">
+      <c r="D40" s="45">
         <v>284</v>
       </c>
     </row>
@@ -25164,10 +25165,10 @@
       <c r="B41" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C41" s="42">
+      <c r="C41" s="41">
         <v>291</v>
       </c>
-      <c r="D41" s="46">
+      <c r="D41" s="45">
         <v>300</v>
       </c>
     </row>
@@ -25178,10 +25179,10 @@
       <c r="B42" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="C42" s="42">
+      <c r="C42" s="41">
         <v>307</v>
       </c>
-      <c r="D42" s="46">
+      <c r="D42" s="45">
         <v>316</v>
       </c>
     </row>
@@ -25192,10 +25193,10 @@
       <c r="B43" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C43" s="42">
+      <c r="C43" s="41">
         <v>196</v>
       </c>
-      <c r="D43" s="42">
+      <c r="D43" s="41">
         <v>207</v>
       </c>
     </row>
@@ -25206,10 +25207,10 @@
       <c r="B44" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="41">
         <v>212</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="41">
         <v>223</v>
       </c>
     </row>
@@ -25220,10 +25221,10 @@
       <c r="B45" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="41">
         <v>228</v>
       </c>
-      <c r="D45" s="46">
+      <c r="D45" s="45">
         <v>239</v>
       </c>
     </row>
@@ -25234,10 +25235,10 @@
       <c r="B46" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C46" s="42">
+      <c r="C46" s="41">
         <v>244</v>
       </c>
-      <c r="D46" s="42">
+      <c r="D46" s="41">
         <v>255</v>
       </c>
     </row>
@@ -25248,10 +25249,10 @@
       <c r="B47" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C47" s="42">
+      <c r="C47" s="41">
         <v>260</v>
       </c>
-      <c r="D47" s="46">
+      <c r="D47" s="45">
         <v>271</v>
       </c>
     </row>
@@ -25262,10 +25263,10 @@
       <c r="B48" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C48" s="42">
+      <c r="C48" s="41">
         <v>276</v>
       </c>
-      <c r="D48" s="46">
+      <c r="D48" s="45">
         <v>287</v>
       </c>
     </row>
@@ -25276,10 +25277,10 @@
       <c r="B49" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C49" s="42">
+      <c r="C49" s="41">
         <v>292</v>
       </c>
-      <c r="D49" s="46">
+      <c r="D49" s="45">
         <v>303</v>
       </c>
     </row>
@@ -25290,10 +25291,10 @@
       <c r="B50" s="13" t="s">
         <v>894</v>
       </c>
-      <c r="C50" s="42">
+      <c r="C50" s="41">
         <v>308</v>
       </c>
-      <c r="D50" s="46">
+      <c r="D50" s="45">
         <v>319</v>
       </c>
     </row>
@@ -26248,7 +26249,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:D50">
+  <autoFilter ref="A1:D50" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="RAD"/>
@@ -26262,7 +26263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>